<commit_message>
beta switch to new sp api setSp implemented
</commit_message>
<xml_diff>
--- a/templates/Inner_Contract.xlsx
+++ b/templates/Inner_Contract.xlsx
@@ -5,51 +5,63 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8477016-F041-48F4-8860-CB7ED13B3D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B299B59E-7546-4317-B405-48107CCF970E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="83" windowWidth="27076" windowHeight="16995" xr2:uid="{1078D20C-27F2-4BD9-B9EF-0CD976B5C671}"/>
+    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{1078D20C-27F2-4BD9-B9EF-0CD976B5C671}"/>
   </bookViews>
   <sheets>
-    <sheet name="Шаблон" sheetId="3" r:id="rId1"/>
+    <sheet name="Contract" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Шаблон!$A$1:$I$74</definedName>
-    <definedName name="Договор_адреса_покупатель">Шаблон!$F$60</definedName>
-    <definedName name="Договор_адреса_покупатель_адрес">Шаблон!$F$61</definedName>
-    <definedName name="Договор_адреса_покупатель_банк">Шаблон!$F$66</definedName>
-    <definedName name="Договор_адреса_покупатель_бик">Шаблон!$F$67</definedName>
-    <definedName name="Договор_адреса_покупатель_должность">Шаблон!$F$72</definedName>
-    <definedName name="Договор_адреса_покупатель_инн">Шаблон!$F$64</definedName>
-    <definedName name="Договор_адреса_покупатель_кс">Шаблон!$F$68</definedName>
-    <definedName name="Договор_адреса_покупатель_огрн">Шаблон!$F$65</definedName>
-    <definedName name="Договор_адреса_покупатель_почта">Шаблон!$F$63</definedName>
-    <definedName name="Договор_адреса_покупатель_рс">Шаблон!$F$69</definedName>
-    <definedName name="Договор_адреса_покупатель_телефон">Шаблон!$F$62</definedName>
-    <definedName name="Договор_адреса_покупатель_фио">Шаблон!$F$74</definedName>
-    <definedName name="Договор_адреса_поставщик">Шаблон!$B$60</definedName>
-    <definedName name="Договор_адреса_поставщик_адрес">Шаблон!$B$61</definedName>
-    <definedName name="Договор_адреса_поставщик_банк">Шаблон!$B$66</definedName>
-    <definedName name="Договор_адреса_поставщик_бик">Шаблон!$B$67</definedName>
-    <definedName name="Договор_адреса_поставщик_должность">Шаблон!$B$72</definedName>
-    <definedName name="Договор_адреса_поставщик_инн">Шаблон!$B$64</definedName>
-    <definedName name="Договор_адреса_поставщик_кс">Шаблон!$B$68</definedName>
-    <definedName name="Договор_адреса_поставщик_огрн">Шаблон!$B$65</definedName>
-    <definedName name="Договор_адреса_поставщик_почта">Шаблон!$B$63</definedName>
-    <definedName name="Договор_адреса_поставщик_рс">Шаблон!$B$69</definedName>
-    <definedName name="Договор_адреса_поставщик_тел">Шаблон!$B$62</definedName>
-    <definedName name="Договор_адреса_поставщик_фио">Шаблон!$B$74</definedName>
-    <definedName name="Договор_дата">Шаблон!$G$2</definedName>
-    <definedName name="Договор_номер">Шаблон!$B$1</definedName>
-    <definedName name="Договор_оплата_дата">Шаблон!$B$24</definedName>
-    <definedName name="Договор_подход_дата">Шаблон!$B$25</definedName>
-    <definedName name="Договор_предмет_массив">Шаблон!$B$8</definedName>
-    <definedName name="Договор_стороны">Шаблон!$B$3</definedName>
-    <definedName name="Договор_цена_всего">Шаблон!$B$21</definedName>
-    <definedName name="Договор_цена_массив">Шаблон!$B$19</definedName>
+    <definedName name="Pg_end">Contract!$H$76</definedName>
+    <definedName name="Pg_start">Contract!$B$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Contract!$A$2:$I$75</definedName>
+    <definedName name="Договор_адреса_заголовок">Contract!$B$59</definedName>
+    <definedName name="Договор_адреса_покупатель">Contract!$F$61</definedName>
+    <definedName name="Договор_адреса_покупатель_адрес">Contract!$F$62</definedName>
+    <definedName name="Договор_адреса_покупатель_банк">Contract!$F$67</definedName>
+    <definedName name="Договор_адреса_покупатель_бик">Contract!$F$68</definedName>
+    <definedName name="Договор_адреса_покупатель_должность">Contract!$F$73</definedName>
+    <definedName name="Договор_адреса_покупатель_инн">Contract!$F$65</definedName>
+    <definedName name="Договор_адреса_покупатель_конец">Contract!$H$61</definedName>
+    <definedName name="Договор_адреса_покупатель_кс">Contract!$F$69</definedName>
+    <definedName name="Договор_адреса_покупатель_огрн">Contract!$F$66</definedName>
+    <definedName name="Договор_адреса_покупатель_почта">Contract!$F$64</definedName>
+    <definedName name="Договор_адреса_покупатель_рс">Contract!$F$70</definedName>
+    <definedName name="Договор_адреса_покупатель_телефон">Contract!$F$63</definedName>
+    <definedName name="Договор_адреса_покупатель_фио">Contract!$F$75</definedName>
+    <definedName name="Договор_адреса_поставщик">Contract!$B$61</definedName>
+    <definedName name="Договор_адреса_поставщик_адрес">Contract!$B$62</definedName>
+    <definedName name="Договор_адреса_поставщик_банк">Contract!$B$67</definedName>
+    <definedName name="Договор_адреса_поставщик_бик">Contract!$B$68</definedName>
+    <definedName name="Договор_адреса_поставщик_должность">Contract!$B$73</definedName>
+    <definedName name="Договор_адреса_поставщик_инн">Contract!$B$65</definedName>
+    <definedName name="Договор_адреса_поставщик_конец">Contract!$C$61</definedName>
+    <definedName name="Договор_адреса_поставщик_кс">Contract!$B$69</definedName>
+    <definedName name="Договор_адреса_поставщик_огрн">Contract!$B$66</definedName>
+    <definedName name="Договор_адреса_поставщик_почта">Contract!$B$64</definedName>
+    <definedName name="Договор_адреса_поставщик_рс">Contract!$B$70</definedName>
+    <definedName name="Договор_адреса_поставщик_тел">Contract!$B$63</definedName>
+    <definedName name="Договор_адреса_поставщик_фио">Contract!$B$75</definedName>
+    <definedName name="Договор_дата">Contract!$G$3</definedName>
+    <definedName name="Договор_доставка">Contract!$B$27</definedName>
+    <definedName name="Договор_качество_конец">Contract!$B$15</definedName>
+    <definedName name="Договор_качество_начало">Contract!$B$11</definedName>
+    <definedName name="Договор_номер">Contract!$B$2</definedName>
+    <definedName name="Договор_оплата_дата">Contract!$B$25</definedName>
+    <definedName name="Договор_подход_дата">Contract!$B$26</definedName>
+    <definedName name="Договор_предмет_массив">Contract!$B$9</definedName>
+    <definedName name="Договор_приемка_товара">Contract!$B$28</definedName>
+    <definedName name="Договор_приемка_товара_качество">Contract!$B$30</definedName>
+    <definedName name="Договор_приемка_товара_количество">Contract!$B$29</definedName>
+    <definedName name="Договор_стороны">Contract!$B$4</definedName>
+    <definedName name="Договор_цена_всего">Contract!$B$22</definedName>
+    <definedName name="Договор_цена_массив">Contract!$B$20</definedName>
+    <definedName name="Договор_цена_начало">Contract!$B$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -72,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="142">
   <si>
     <t>ДОГОВОР ПОСТАВКИ № 551</t>
   </si>
@@ -966,6 +978,9 @@
   </si>
   <si>
     <t>Тел. (423) 225-10-68. Факс 89089942222</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1149,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1149,9 +1164,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1229,7 +1241,65 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
@@ -1240,108 +1310,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="3"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1681,910 +1672,852 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H74"/>
+  <dimension ref="B1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A49" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65:C65"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="1.59765625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="39" style="8" customWidth="1"/>
-    <col min="3" max="3" width="15" style="8" customWidth="1"/>
-    <col min="4" max="4" width="11.1328125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="9.265625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="29.59765625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="15.265625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="8.19921875" style="8" customWidth="1"/>
-    <col min="9" max="9" width="2.06640625" style="8" customWidth="1"/>
-    <col min="10" max="16384" width="9.06640625" style="8"/>
+    <col min="1" max="1" width="1.59765625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="39" style="7" customWidth="1"/>
+    <col min="3" max="3" width="15" style="7" customWidth="1"/>
+    <col min="4" max="4" width="11.1328125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.265625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="29.59765625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="15.265625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="8.19921875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="2.06640625" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="23.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="50" t="s">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B1" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="23.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="6"/>
-    </row>
-    <row r="2" spans="2:8" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+    </row>
+    <row r="3" spans="2:8" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="G2" s="35" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="G3" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="35"/>
-    </row>
-    <row r="3" spans="2:8" ht="68.349999999999994" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="34" t="s">
+      <c r="H3" s="54"/>
+    </row>
+    <row r="4" spans="2:8" ht="68.349999999999994" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-    </row>
-    <row r="4" spans="2:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="2:8" s="10" customFormat="1" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="33" t="s">
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+    </row>
+    <row r="5" spans="2:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="2:8" s="9" customFormat="1" ht="12.85" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="6" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="36" t="s">
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+    </row>
+    <row r="7" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-    </row>
-    <row r="7" spans="2:8" s="11" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="25" t="s">
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+    </row>
+    <row r="8" spans="2:8" s="10" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C8" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="26" t="s">
+      <c r="D8" s="47"/>
+      <c r="E8" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F8" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="G7" s="40" t="s">
+      <c r="G8" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="H7" s="41"/>
-    </row>
-    <row r="8" spans="2:8" s="11" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="21" t="s">
+      <c r="H8" s="50"/>
+    </row>
+    <row r="9" spans="2:8" s="10" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C9" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="D8" s="42"/>
-      <c r="E8" s="22" t="s">
+      <c r="D9" s="48"/>
+      <c r="E9" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F9" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="G8" s="42" t="s">
+      <c r="G9" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="H8" s="43"/>
-    </row>
-    <row r="9" spans="2:8" s="12" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="23" t="s">
+      <c r="H9" s="51"/>
+    </row>
+    <row r="10" spans="2:8" s="11" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="44" t="s">
+      <c r="C10" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="24" t="s">
+      <c r="D10" s="49"/>
+      <c r="E10" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F10" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="G9" s="44" t="s">
+      <c r="G10" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="H9" s="45"/>
-    </row>
-    <row r="10" spans="2:8" ht="35.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="47" t="s">
+      <c r="H10" s="52"/>
+    </row>
+    <row r="11" spans="2:8" ht="35.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-    </row>
-    <row r="11" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="39" t="s">
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+    </row>
+    <row r="12" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-    </row>
-    <row r="12" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="39" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+    </row>
+    <row r="13" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-    </row>
-    <row r="13" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="48" t="s">
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-    </row>
-    <row r="14" spans="2:8" ht="23.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="49" t="s">
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="2:8" ht="23.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="49"/>
-    </row>
-    <row r="15" spans="2:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="2:8" ht="14.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="52" t="s">
+    </row>
+    <row r="16" spans="2:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" spans="2:8" ht="14.65" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="2:8" ht="22.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="28" t="s">
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="2:8" ht="22.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="2:8" s="12" customFormat="1" ht="26.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="25" t="s">
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="2:8" s="11" customFormat="1" ht="26.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C19" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="40"/>
-      <c r="E18" s="26" t="s">
+      <c r="D19" s="47"/>
+      <c r="E19" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="F18" s="26" t="s">
+      <c r="F19" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="26" t="s">
+      <c r="G19" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="H18" s="27" t="s">
+      <c r="H19" s="26" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="2:8" s="12" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="21" t="s">
+    <row r="20" spans="2:8" s="11" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C20" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="42"/>
-      <c r="E19" s="22" t="s">
+      <c r="D20" s="48"/>
+      <c r="E20" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="29" t="s">
+      <c r="F20" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G20" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="H19" s="31">
+      <c r="H20" s="30">
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="2:8" s="12" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="23" t="s">
+    <row r="21" spans="2:8" s="11" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C21" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="44"/>
-      <c r="E20" s="24" t="s">
+      <c r="D21" s="49"/>
+      <c r="E21" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="F21" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="G20" s="24" t="s">
+      <c r="G21" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="H20" s="32">
+      <c r="H21" s="31">
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="2:8" s="11" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="46" t="s">
+    <row r="22" spans="2:8" s="10" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-    </row>
-    <row r="22" spans="2:8" s="11" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B23" s="50" t="s">
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+    </row>
+    <row r="23" spans="2:8" s="10" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B24" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="2:8" ht="39.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="39" t="s">
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="2:8" ht="39.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-    </row>
-    <row r="25" spans="2:8" s="12" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="39" t="s">
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+    </row>
+    <row r="26" spans="2:8" s="11" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-    </row>
-    <row r="26" spans="2:8" s="12" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="39" t="s">
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+    </row>
+    <row r="27" spans="2:8" s="11" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-    </row>
-    <row r="27" spans="2:8" s="58" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="59" t="s">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+    </row>
+    <row r="28" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
-    </row>
-    <row r="28" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="51" t="s">
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+    </row>
+    <row r="29" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-    </row>
-    <row r="29" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="37" t="s">
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+    </row>
+    <row r="30" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-    </row>
-    <row r="30" spans="2:8" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="39" t="s">
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+    </row>
+    <row r="31" spans="2:8" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-    </row>
-    <row r="31" spans="2:8" s="12" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="39" t="s">
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+    </row>
+    <row r="32" spans="2:8" s="11" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-    </row>
-    <row r="32" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="48" t="s">
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+    </row>
+    <row r="33" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
-    </row>
-    <row r="33" spans="2:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B34" s="50" t="s">
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+    </row>
+    <row r="34" spans="2:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B35" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="6"/>
-    </row>
-    <row r="35" spans="2:8" ht="16.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="38" t="s">
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+    </row>
+    <row r="36" spans="2:8" ht="16.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B36" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
-      <c r="G35" s="38"/>
-      <c r="H35" s="38"/>
-    </row>
-    <row r="36" spans="2:8" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="38" t="s">
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+    </row>
+    <row r="37" spans="2:8" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="38"/>
-    </row>
-    <row r="37" spans="2:8" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="38" t="s">
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+    </row>
+    <row r="38" spans="2:8" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-    </row>
-    <row r="38" spans="2:8" ht="56.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="38" t="s">
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+    </row>
+    <row r="39" spans="2:8" ht="56.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B39" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
-    </row>
-    <row r="39" spans="2:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="38" t="s">
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+    </row>
+    <row r="40" spans="2:8" ht="82.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B40" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="38"/>
-    </row>
-    <row r="40" spans="2:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B41" s="50" t="s">
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+    </row>
+    <row r="41" spans="2:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B42" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="6"/>
-    </row>
-    <row r="42" spans="2:8" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="38" t="s">
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+    </row>
+    <row r="43" spans="2:8" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="38"/>
-    </row>
-    <row r="43" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="39" t="s">
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+    </row>
+    <row r="44" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B44" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39"/>
-    </row>
-    <row r="44" spans="2:8" ht="26.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="38" t="s">
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+    </row>
+    <row r="45" spans="2:8" ht="26.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B45" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="38"/>
-    </row>
-    <row r="45" spans="2:8" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="38" t="s">
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+    </row>
+    <row r="46" spans="2:8" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B46" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-    </row>
-    <row r="46" spans="2:8" ht="40.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="38" t="s">
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+    </row>
+    <row r="47" spans="2:8" ht="40.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B47" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-    </row>
-    <row r="47" spans="2:8" ht="30.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="38" t="s">
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+    </row>
+    <row r="48" spans="2:8" ht="30.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B48" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-    </row>
-    <row r="48" spans="2:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B49" s="50" t="s">
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+    </row>
+    <row r="49" spans="2:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B50" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C49" s="50"/>
-      <c r="D49" s="50"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="50"/>
-      <c r="G49" s="50"/>
-      <c r="H49" s="6"/>
-    </row>
-    <row r="50" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="38" t="s">
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+    </row>
+    <row r="51" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B51" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="38"/>
-    </row>
-    <row r="51" spans="2:8" s="20" customFormat="1" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="39" t="s">
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+    </row>
+    <row r="52" spans="2:8" s="19" customFormat="1" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B52" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="C51" s="39"/>
-      <c r="D51" s="39"/>
-      <c r="E51" s="39"/>
-      <c r="F51" s="39"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="39"/>
-    </row>
-    <row r="52" spans="2:8" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="39" t="s">
+    </row>
+    <row r="53" spans="2:8" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B53" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C52" s="39"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="39"/>
-      <c r="F52" s="39"/>
-      <c r="G52" s="39"/>
-      <c r="H52" s="39"/>
-    </row>
-    <row r="53" spans="2:8" s="12" customFormat="1" ht="40.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="38" t="s">
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+    </row>
+    <row r="54" spans="2:8" s="11" customFormat="1" ht="40.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B54" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-    </row>
-    <row r="54" spans="2:8" s="4" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B54" s="39" t="s">
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+    </row>
+    <row r="55" spans="2:8" s="4" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B55" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="39"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="39"/>
-      <c r="F54" s="39"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="39"/>
-    </row>
-    <row r="55" spans="2:8" s="9" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="38" t="s">
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+    </row>
+    <row r="56" spans="2:8" s="8" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B56" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C55" s="38"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="38"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="38"/>
-      <c r="H55" s="38"/>
-    </row>
-    <row r="56" spans="2:8" s="12" customFormat="1" ht="44.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="38" t="s">
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+    </row>
+    <row r="57" spans="2:8" s="11" customFormat="1" ht="44.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B57" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C56" s="38"/>
-      <c r="D56" s="38"/>
-      <c r="E56" s="38"/>
-      <c r="F56" s="38"/>
-      <c r="G56" s="38"/>
-      <c r="H56" s="38"/>
-    </row>
-    <row r="57" spans="2:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="58" spans="2:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="33" t="s">
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+    </row>
+    <row r="58" spans="2:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="59" spans="2:8" s="9" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B59" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C58" s="33"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="33"/>
-      <c r="F58" s="33"/>
-      <c r="G58" s="33"/>
-      <c r="H58" s="33"/>
-    </row>
-    <row r="59" spans="2:8" s="10" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B59" s="16"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="16"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16"/>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B60" s="60" t="s">
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+    </row>
+    <row r="60" spans="2:8" s="9" customFormat="1" ht="10.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+    </row>
+    <row r="61" spans="2:8" ht="25.5" x14ac:dyDescent="0.4">
+      <c r="B61" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="60"/>
-      <c r="D60" s="57"/>
-      <c r="F60" s="64" t="s">
+      <c r="C61" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="D61" s="32"/>
+      <c r="F61" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="G60" s="64"/>
-      <c r="H60" s="64"/>
-    </row>
-    <row r="61" spans="2:8" ht="24.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B61" s="61" t="s">
+      <c r="G61" s="14"/>
+      <c r="H61" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" ht="24.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B62" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="61"/>
-      <c r="D61" s="17"/>
-      <c r="F61" s="65" t="s">
+      <c r="C62" s="16"/>
+      <c r="D62" s="16"/>
+      <c r="F62" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="G61" s="65"/>
-      <c r="H61" s="65"/>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B62" s="61" t="s">
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+    </row>
+    <row r="63" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B63" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="61"/>
-      <c r="D62" s="17"/>
-      <c r="F62" s="66" t="s">
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="F63" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="G62" s="66"/>
-      <c r="H62" s="66"/>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B63" s="62" t="s">
+      <c r="G63" s="16"/>
+      <c r="H63" s="16"/>
+    </row>
+    <row r="64" spans="2:8" ht="12.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B64" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C63" s="62"/>
-      <c r="D63" s="17"/>
-      <c r="F63" s="66" t="s">
+      <c r="C64" s="63"/>
+      <c r="D64" s="16"/>
+      <c r="F64" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="G63" s="66"/>
-      <c r="H63" s="66"/>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B64" s="61" t="s">
+      <c r="G64" s="16"/>
+      <c r="H64" s="16"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B65" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="C64" s="61"/>
-      <c r="D64" s="17"/>
-      <c r="F64" s="66" t="s">
+      <c r="C65" s="16"/>
+      <c r="D65" s="16"/>
+      <c r="F65" s="41" t="s">
         <v>139</v>
       </c>
-      <c r="G64" s="66"/>
-      <c r="H64" s="66"/>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B65" s="61" t="s">
+      <c r="G65" s="16"/>
+      <c r="H65" s="16"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B66" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="C65" s="61"/>
-      <c r="D65" s="18"/>
-      <c r="F65" s="66" t="s">
+      <c r="C66" s="16"/>
+      <c r="D66" s="17"/>
+      <c r="F66" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="G65" s="66"/>
-      <c r="H65" s="66"/>
-    </row>
-    <row r="66" spans="2:8" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B66" s="63" t="s">
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
+    </row>
+    <row r="67" spans="2:8" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B67" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="C66" s="63"/>
-      <c r="F66" s="65" t="s">
+      <c r="C67" s="11"/>
+      <c r="F67" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="G66" s="65"/>
-      <c r="H66" s="65"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B67" s="61" t="s">
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B68" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C67" s="61"/>
-      <c r="D67" s="17"/>
-      <c r="F67" s="66" t="s">
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
+      <c r="F68" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="G67" s="66"/>
-      <c r="H67" s="66"/>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B68" s="61" t="s">
+      <c r="G68" s="16"/>
+      <c r="H68" s="16"/>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B69" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C68" s="61"/>
-      <c r="D68" s="17"/>
-      <c r="F68" s="66" t="s">
+      <c r="C69" s="16"/>
+      <c r="D69" s="16"/>
+      <c r="F69" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="G68" s="66"/>
-      <c r="H68" s="66"/>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B69" s="61" t="s">
+      <c r="G69" s="16"/>
+      <c r="H69" s="16"/>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B70" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C69" s="61"/>
-      <c r="D69" s="17"/>
-      <c r="F69" s="66" t="s">
+      <c r="C70" s="16"/>
+      <c r="D70" s="16"/>
+      <c r="F70" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="G69" s="66"/>
-      <c r="H69" s="66"/>
-    </row>
-    <row r="71" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B72" s="68" t="s">
+      <c r="G70" s="16"/>
+      <c r="H70" s="16"/>
+    </row>
+    <row r="72" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B73" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="C72" s="68"/>
-      <c r="D72" s="19"/>
-      <c r="F72" s="64" t="s">
+      <c r="C73" s="46"/>
+      <c r="D73" s="18"/>
+      <c r="F73" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="G72" s="64"/>
-      <c r="H72" s="64"/>
-    </row>
-    <row r="73" spans="2:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B73" s="69"/>
-      <c r="C73" s="67"/>
-      <c r="F73" s="70"/>
-      <c r="G73" s="70"/>
-      <c r="H73" s="70"/>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B74" s="68" t="s">
+      <c r="G73" s="44"/>
+      <c r="H73" s="44"/>
+    </row>
+    <row r="74" spans="2:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B74" s="34"/>
+      <c r="C74" s="33"/>
+      <c r="F74" s="35"/>
+      <c r="G74" s="35"/>
+      <c r="H74" s="35"/>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B75" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="C74" s="68"/>
-      <c r="D74" s="19"/>
-      <c r="F74" s="71" t="s">
+      <c r="C75" s="46"/>
+      <c r="D75" s="18"/>
+      <c r="F75" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="G74" s="71"/>
-      <c r="H74" s="71"/>
+      <c r="G75" s="45"/>
+      <c r="H75" s="45"/>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="H76" s="7" t="s">
+        <v>141</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="77">
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="C7:D7"/>
+  <mergeCells count="18">
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B75:C75"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F60:H60"/>
-    <mergeCell ref="F61:H61"/>
-    <mergeCell ref="F62:H62"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B56:H56"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B46:H46"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="G7:H7"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="G9:H9"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B41:G41"/>
-    <mergeCell ref="B34:G34"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B58:H58"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B50:H50"/>
-    <mergeCell ref="B51:H51"/>
-    <mergeCell ref="B52:H52"/>
-    <mergeCell ref="B53:H53"/>
-    <mergeCell ref="B54:H54"/>
-    <mergeCell ref="B55:H55"/>
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="B37:H37"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="G3:H3"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B63" r:id="rId1" display="mailto:main@sea-wolf.ru" xr:uid="{05169D76-8F73-4774-BE32-CF7029FF34EB}"/>
-  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="7.874015748031496E-2" right="7.874015748031496E-2" top="0.19685039370078741" bottom="0.19685039370078741" header="0.11811023622047245" footer="0"/>
-  <pageSetup paperSize="9" scale="79" fitToHeight="2" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="79" fitToHeight="2" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="37" max="7" man="1"/>
+    <brk id="38" max="7" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -2599,22 +2532,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="1.59765625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="9.265625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="47.19921875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="2.06640625" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="9.06640625" style="8"/>
+    <col min="1" max="1" width="1.59765625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="9.265625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="47.19921875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="2.06640625" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="9.06640625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="23.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-    </row>
-    <row r="2" spans="2:4" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+    </row>
+    <row r="2" spans="2:4" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2623,479 +2556,452 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="99.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
     </row>
     <row r="5" spans="2:4" ht="26.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-    </row>
-    <row r="6" spans="2:4" s="11" customFormat="1" ht="35.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="54" t="s">
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+    </row>
+    <row r="6" spans="2:4" s="10" customFormat="1" ht="35.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-    </row>
-    <row r="7" spans="2:4" s="12" customFormat="1" ht="35.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="54" t="s">
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+    </row>
+    <row r="7" spans="2:4" s="11" customFormat="1" ht="35.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="60"/>
     </row>
     <row r="9" spans="2:4" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="2:4" ht="14.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:4" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="54" t="s">
+    <row r="12" spans="2:4" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-    </row>
-    <row r="13" spans="2:4" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="54" t="s">
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+    </row>
+    <row r="13" spans="2:4" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-    </row>
-    <row r="14" spans="2:4" s="11" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="54" t="s">
+      <c r="C13" s="57"/>
+      <c r="D13" s="57"/>
+    </row>
+    <row r="14" spans="2:4" s="10" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
     </row>
     <row r="16" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
     </row>
     <row r="17" spans="2:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
     </row>
     <row r="18" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="54" t="s">
+      <c r="B18" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B19" s="54" t="s">
+      <c r="B19" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="60"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
     </row>
     <row r="24" spans="2:4" ht="39.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-    </row>
-    <row r="25" spans="2:4" s="12" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="54" t="s">
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+    </row>
+    <row r="25" spans="2:4" s="11" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-    </row>
-    <row r="26" spans="2:4" s="12" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="54" t="s">
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+    </row>
+    <row r="26" spans="2:4" s="11" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
     </row>
     <row r="27" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="54" t="s">
+      <c r="B27" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-    </row>
-    <row r="30" spans="2:4" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="54" t="s">
+      <c r="C29" s="60"/>
+      <c r="D29" s="60"/>
+    </row>
+    <row r="30" spans="2:4" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="54"/>
-    </row>
-    <row r="31" spans="2:4" s="12" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="54" t="s">
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+    </row>
+    <row r="31" spans="2:4" s="11" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="54"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="60"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
     </row>
     <row r="35" spans="2:4" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
     </row>
     <row r="36" spans="2:4" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="54" t="s">
+      <c r="B36" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
     </row>
     <row r="37" spans="2:4" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="54" t="s">
+      <c r="B37" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="54"/>
-      <c r="D37" s="54"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
     </row>
     <row r="38" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="56" t="s">
+      <c r="B38" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="59"/>
     </row>
     <row r="39" spans="2:4" ht="113.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="53" t="s">
+      <c r="B39" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="58"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-    </row>
-    <row r="42" spans="2:4" s="9" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="54" t="s">
+      <c r="C41" s="43"/>
+      <c r="D41" s="43"/>
+    </row>
+    <row r="42" spans="2:4" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B42" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="54"/>
-      <c r="D42" s="54"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="57"/>
     </row>
     <row r="43" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="54" t="s">
+      <c r="B43" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="54"/>
-      <c r="D43" s="54"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="57"/>
     </row>
     <row r="44" spans="2:4" ht="30.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="53" t="s">
+      <c r="B44" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="58"/>
     </row>
     <row r="45" spans="2:4" ht="42.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="53" t="s">
+      <c r="B45" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="53"/>
-      <c r="D45" s="53"/>
+      <c r="C45" s="58"/>
+      <c r="D45" s="58"/>
     </row>
     <row r="46" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="53" t="s">
+      <c r="B46" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="53"/>
-      <c r="D46" s="53"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
     </row>
     <row r="47" spans="2:4" ht="39" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="53" t="s">
+      <c r="B47" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="58"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="50"/>
-      <c r="D49" s="50"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B50" s="53" t="s">
+      <c r="B50" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="53"/>
-      <c r="D50" s="53"/>
-    </row>
-    <row r="51" spans="2:4" s="13" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="53" t="s">
+      <c r="C50" s="58"/>
+      <c r="D50" s="58"/>
+    </row>
+    <row r="51" spans="2:4" s="12" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B51" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="53"/>
-      <c r="D51" s="53"/>
+      <c r="C51" s="58"/>
+      <c r="D51" s="58"/>
     </row>
     <row r="52" spans="2:4" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="54" t="s">
+      <c r="B52" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="54"/>
-      <c r="D52" s="54"/>
-    </row>
-    <row r="53" spans="2:4" s="12" customFormat="1" ht="36.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="54" t="s">
+      <c r="C52" s="57"/>
+      <c r="D52" s="57"/>
+    </row>
+    <row r="53" spans="2:4" s="11" customFormat="1" ht="36.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B53" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="54"/>
-      <c r="D53" s="54"/>
-    </row>
-    <row r="54" spans="2:4" s="9" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B54" s="53" t="s">
+      <c r="C53" s="57"/>
+      <c r="D53" s="57"/>
+    </row>
+    <row r="54" spans="2:4" s="8" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B54" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="53"/>
-      <c r="D54" s="53"/>
-    </row>
-    <row r="55" spans="2:4" s="9" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="54" t="s">
+      <c r="C54" s="58"/>
+      <c r="D54" s="58"/>
+    </row>
+    <row r="55" spans="2:4" s="8" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B55" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="54"/>
-      <c r="D55" s="54"/>
-    </row>
-    <row r="56" spans="2:4" s="12" customFormat="1" ht="51.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="54" t="s">
+      <c r="C55" s="57"/>
+      <c r="D55" s="57"/>
+    </row>
+    <row r="56" spans="2:4" s="11" customFormat="1" ht="51.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B56" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="54"/>
-      <c r="D56" s="54"/>
-    </row>
-    <row r="58" spans="2:4" s="10" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="33" t="s">
+      <c r="C56" s="57"/>
+      <c r="D56" s="57"/>
+    </row>
+    <row r="58" spans="2:4" s="9" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B58" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="33"/>
-      <c r="D58" s="33"/>
+      <c r="C58" s="56"/>
+      <c r="D58" s="56"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D59" s="15" t="s">
+      <c r="D59" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D60" s="8" t="s">
+      <c r="D60" s="7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D61" s="17" t="s">
+      <c r="D61" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B62" s="17" t="s">
+      <c r="B62" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="D62" s="17" t="s">
+      <c r="D62" s="16" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B63" s="17" t="s">
+      <c r="B63" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D63" s="17" t="s">
+      <c r="D63" s="16" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B64" s="18" t="s">
+      <c r="B64" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D64" s="17" t="s">
+      <c r="D64" s="16" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B65" s="8" t="s">
+      <c r="B65" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D65" s="17" t="s">
+      <c r="D65" s="16" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B66" s="17" t="s">
+      <c r="B66" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D66" s="17" t="s">
+      <c r="D66" s="16" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B67" s="17" t="s">
+      <c r="B67" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="D67" s="17" t="s">
+      <c r="D67" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B68" s="17" t="s">
+      <c r="B68" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D68" s="17" t="s">
+      <c r="D68" s="16" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="70" spans="2:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="71" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B71" s="19" t="s">
+      <c r="B71" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D71" s="15" t="s">
+      <c r="D71" s="14" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="72" spans="2:4" ht="19.25" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="73" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B73" s="19" t="s">
+      <c r="B73" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D73" s="19" t="s">
+      <c r="D73" s="18" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B3:D3"/>
@@ -3108,11 +3014,38 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B64" r:id="rId1" display="mailto:main@sea-wolf.ru" xr:uid="{65C32F44-9D5B-4BC8-B696-A4811EE9907B}"/>

</xml_diff>

<commit_message>
request fixed, inner contract in development, need to fix initrows last cell border disappear on merge cells
</commit_message>
<xml_diff>
--- a/templates/Inner_Contract.xlsx
+++ b/templates/Inner_Contract.xlsx
@@ -8,58 +8,64 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4986592F-E6FD-4CAC-939E-F7C16DFDCCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAFE533-7346-4392-9DCC-A73EA6B62E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57697" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{1078D20C-27F2-4BD9-B9EF-0CD976B5C671}"/>
+    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{1078D20C-27F2-4BD9-B9EF-0CD976B5C671}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Pg_end">Contract!$H$77</definedName>
+    <definedName name="Pg_end">Contract!$H$81</definedName>
     <definedName name="Pg_start">Contract!$B$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Contract!$A$2:$I$76</definedName>
-    <definedName name="Договор_адреса_заголовок">Contract!$B$61</definedName>
-    <definedName name="Договор_адреса_покупатель">Contract!$F$62</definedName>
-    <definedName name="Договор_адреса_покупатель_адрес">Contract!$F$63</definedName>
-    <definedName name="Договор_адреса_покупатель_банк">Contract!$F$68</definedName>
-    <definedName name="Договор_адреса_покупатель_бик">Contract!$F$69</definedName>
-    <definedName name="Договор_адреса_покупатель_должность">Contract!$F$74</definedName>
-    <definedName name="Договор_адреса_покупатель_инн">Contract!$F$66</definedName>
-    <definedName name="Договор_адреса_покупатель_конец">Contract!$H$62</definedName>
-    <definedName name="Договор_адреса_покупатель_кс">Contract!$F$70</definedName>
-    <definedName name="Договор_адреса_покупатель_огрн">Contract!$F$67</definedName>
-    <definedName name="Договор_адреса_покупатель_почта">Contract!$F$65</definedName>
-    <definedName name="Договор_адреса_покупатель_рс">Contract!$F$71</definedName>
-    <definedName name="Договор_адреса_покупатель_тел">Contract!$F$64</definedName>
-    <definedName name="Договор_адреса_покупатель_фио">Contract!$F$76</definedName>
-    <definedName name="Договор_адреса_поставщик">Contract!$B$62</definedName>
-    <definedName name="Договор_адреса_поставщик_адрес">Contract!$B$63</definedName>
-    <definedName name="Договор_адреса_поставщик_банк">Contract!$B$68</definedName>
-    <definedName name="Договор_адреса_поставщик_бик">Contract!$B$69</definedName>
-    <definedName name="Договор_адреса_поставщик_должность">Contract!$B$74</definedName>
-    <definedName name="Договор_адреса_поставщик_инн">Contract!$B$66</definedName>
-    <definedName name="Договор_адреса_поставщик_конец">Contract!$C$62</definedName>
-    <definedName name="Договор_адреса_поставщик_кс">Contract!$B$70</definedName>
-    <definedName name="Договор_адреса_поставщик_огрн">Contract!$B$67</definedName>
-    <definedName name="Договор_адреса_поставщик_почта">Contract!$B$65</definedName>
-    <definedName name="Договор_адреса_поставщик_рс">Contract!$B$71</definedName>
-    <definedName name="Договор_адреса_поставщик_тел">Contract!$B$64</definedName>
-    <definedName name="Договор_адреса_поставщик_фио">Contract!$B$76</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Contract!$A$2:$I$80</definedName>
+    <definedName name="Договор_адреса_заголовок">Contract!$B$65</definedName>
+    <definedName name="Договор_адреса_покупатель">Contract!$F$66</definedName>
+    <definedName name="Договор_адреса_покупатель_адрес">Contract!$F$67</definedName>
+    <definedName name="Договор_адреса_покупатель_банк">Contract!$F$72</definedName>
+    <definedName name="Договор_адреса_покупатель_бик">Contract!$F$73</definedName>
+    <definedName name="Договор_адреса_покупатель_должность">Contract!$F$78</definedName>
+    <definedName name="Договор_адреса_покупатель_инн">Contract!$F$70</definedName>
+    <definedName name="Договор_адреса_покупатель_конец">Contract!$H$66</definedName>
+    <definedName name="Договор_адреса_покупатель_кс">Contract!$F$74</definedName>
+    <definedName name="Договор_адреса_покупатель_огрн">Contract!$F$71</definedName>
+    <definedName name="Договор_адреса_покупатель_почта">Contract!$F$69</definedName>
+    <definedName name="Договор_адреса_покупатель_рс">Contract!$F$75</definedName>
+    <definedName name="Договор_адреса_покупатель_тел">Contract!$F$68</definedName>
+    <definedName name="Договор_адреса_покупатель_фио">Contract!$F$80</definedName>
+    <definedName name="Договор_адреса_поставщик">Contract!$B$66</definedName>
+    <definedName name="Договор_адреса_поставщик_адрес">Contract!$B$67</definedName>
+    <definedName name="Договор_адреса_поставщик_банк">Contract!$B$72</definedName>
+    <definedName name="Договор_адреса_поставщик_бик">Contract!$B$73</definedName>
+    <definedName name="Договор_адреса_поставщик_должность">Contract!$B$78</definedName>
+    <definedName name="Договор_адреса_поставщик_инн">Contract!$B$70</definedName>
+    <definedName name="Договор_адреса_поставщик_конец">Contract!$C$66</definedName>
+    <definedName name="Договор_адреса_поставщик_кс">Contract!$B$74</definedName>
+    <definedName name="Договор_адреса_поставщик_огрн">Contract!$B$71</definedName>
+    <definedName name="Договор_адреса_поставщик_почта">Contract!$B$69</definedName>
+    <definedName name="Договор_адреса_поставщик_рс">Contract!$B$75</definedName>
+    <definedName name="Договор_адреса_поставщик_тел">Contract!$B$68</definedName>
+    <definedName name="Договор_адреса_поставщик_фио">Contract!$B$80</definedName>
     <definedName name="Договор_дата">Contract!$G$3</definedName>
-    <definedName name="Договор_доставка">Contract!$B$29</definedName>
+    <definedName name="Договор_доставка">Contract!$B$33</definedName>
     <definedName name="Договор_качество_конец">Contract!#REF!</definedName>
     <definedName name="Договор_качество_начало">Contract!#REF!</definedName>
     <definedName name="Договор_конец_предмет">Contract!$B$11</definedName>
+    <definedName name="Договор_Меркурий">Contract!$B$39</definedName>
+    <definedName name="Договор_Меркурий_EXW">Contract!$B$31</definedName>
+    <definedName name="Договор_момент_приемки">Contract!$B$37</definedName>
+    <definedName name="Договор_момент_приемки_EXW">Contract!$B$30</definedName>
     <definedName name="Договор_номер">Contract!$B$2</definedName>
     <definedName name="Договор_оплата_дата">Contract!$B$27</definedName>
-    <definedName name="Договор_подход_дата">Contract!$B$28</definedName>
+    <definedName name="Договор_передача_EXW">Contract!$B$28</definedName>
+    <definedName name="Договор_подход_дата">Contract!$B$32</definedName>
     <definedName name="Договор_предмет_массив">Contract!$B$9</definedName>
-    <definedName name="Договор_приемка_товара">Contract!$B$30</definedName>
-    <definedName name="Договор_приемка_товара_ВСД">Contract!$B$34</definedName>
-    <definedName name="Договор_приемка_товара_качество">Contract!$B$32</definedName>
-    <definedName name="Договор_приемка_товара_количество">Contract!$B$31</definedName>
+    <definedName name="Договор_приемка_EXW">Contract!$B$29</definedName>
+    <definedName name="Договор_приемка_товара">Contract!$B$34</definedName>
+    <definedName name="Договор_приемка_товара_ВСД">Contract!$B$38</definedName>
+    <definedName name="Договор_приемка_товара_качество">Contract!$B$36</definedName>
+    <definedName name="Договор_приемка_товара_количество">Contract!$B$35</definedName>
     <definedName name="Договор_стороны">Contract!$B$4</definedName>
     <definedName name="Договор_цена_всего">Contract!$B$18</definedName>
     <definedName name="Договор_цена_массив">Contract!$B$16</definedName>
@@ -86,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="115">
   <si>
     <t>ДОГОВОР ПОСТАВКИ № 551</t>
   </si>
@@ -886,6 +892,18 @@
       </rPr>
       <t>18-20 декабря 2023 года.</t>
     </r>
+  </si>
+  <si>
+    <t>4.2. Товар передается Покупателю с холодильника в порту Владивосток после внесения предоплаты. Грузовые работы с холодильника в порту Владивосток – за счет Покупателя.</t>
+  </si>
+  <si>
+    <t>4.3. Приемка товара по качеству и количеству осуществляется Покупателем или его уполномоченным представителем на холодильнике в порту Владивосток в момент получения товара.</t>
+  </si>
+  <si>
+    <t>4.4. С момента приемки товара по количеству и качеству, согласно п. 4.3 настоящего договора, в дальнейшем никакие претензии по количеству и качеству товара от Покупателя Поставщиком не принимаются.</t>
+  </si>
+  <si>
+    <t>4.5. Покупатель обязан подтвердить регистрацию в ГИС «Меркурий».</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1095,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1117,30 +1135,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1152,29 +1146,17 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1188,9 +1170,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1206,9 +1185,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1223,11 +1199,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1236,78 +1209,119 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1647,840 +1661,881 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H77"/>
+  <dimension ref="B1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="148" zoomScaleNormal="100" zoomScaleSheetLayoutView="148" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="1.59765625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="39" style="23" customWidth="1"/>
-    <col min="3" max="3" width="15" style="23" customWidth="1"/>
-    <col min="4" max="4" width="10.265625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="6.59765625" style="23" customWidth="1"/>
-    <col min="6" max="6" width="32.59765625" style="23" customWidth="1"/>
-    <col min="7" max="7" width="11.19921875" style="23" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="23" customWidth="1"/>
-    <col min="9" max="9" width="2.06640625" style="23" customWidth="1"/>
-    <col min="10" max="16384" width="9.06640625" style="23"/>
+    <col min="1" max="1" width="1.59765625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="39" style="15" customWidth="1"/>
+    <col min="3" max="3" width="15" style="15" customWidth="1"/>
+    <col min="4" max="4" width="10.265625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="6.59765625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="32.59765625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="15" customWidth="1"/>
+    <col min="9" max="9" width="2.06640625" style="15" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="15" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="2" spans="2:8" ht="23.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-    </row>
-    <row r="3" spans="2:8" s="26" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="25" t="s">
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+    </row>
+    <row r="3" spans="2:8" s="18" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="G3" s="27" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="G3" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="27"/>
+      <c r="H3" s="66"/>
     </row>
     <row r="4" spans="2:8" ht="66" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
     </row>
     <row r="5" spans="2:8" ht="5.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-    </row>
-    <row r="6" spans="2:8" s="26" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="30" t="s">
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+    </row>
+    <row r="6" spans="2:8" s="18" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
     </row>
     <row r="7" spans="2:8" ht="29.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="2:8" s="36" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="32" t="s">
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+    </row>
+    <row r="8" spans="2:8" s="24" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="34" t="s">
+      <c r="D8" s="61"/>
+      <c r="E8" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="33" t="s">
+      <c r="G8" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="35"/>
-    </row>
-    <row r="9" spans="2:8" s="36" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="37" t="s">
+      <c r="H8" s="64"/>
+    </row>
+    <row r="9" spans="2:8" s="24" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="39" t="s">
+      <c r="D9" s="62"/>
+      <c r="E9" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="G9" s="41" t="s">
+      <c r="G9" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="H9" s="42"/>
-    </row>
-    <row r="10" spans="2:8" s="49" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="43" t="s">
+      <c r="H9" s="29"/>
+    </row>
+    <row r="10" spans="2:8" s="35" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="45" t="s">
+      <c r="D10" s="63"/>
+      <c r="E10" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="46" t="s">
+      <c r="F10" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="47" t="s">
+      <c r="G10" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="H10" s="48"/>
+      <c r="H10" s="34"/>
     </row>
     <row r="11" spans="2:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
     </row>
     <row r="12" spans="2:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="51"/>
+      <c r="B12" s="37"/>
     </row>
     <row r="13" spans="2:8" ht="14.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="52" t="s">
+      <c r="B13" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
     </row>
     <row r="14" spans="2:8" ht="22.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="55"/>
-    </row>
-    <row r="15" spans="2:8" s="49" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="32" t="s">
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="40"/>
+    </row>
+    <row r="15" spans="2:8" s="35" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="34" t="s">
+      <c r="D15" s="61"/>
+      <c r="E15" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="34" t="s">
+      <c r="F15" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="G15" s="34" t="s">
+      <c r="G15" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="H15" s="56" t="s">
+      <c r="H15" s="23" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="2:8" s="49" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="37" t="s">
+    <row r="16" spans="2:8" s="35" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="38"/>
-      <c r="E16" s="39" t="s">
+      <c r="D16" s="62"/>
+      <c r="E16" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="F16" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="39" t="s">
+      <c r="G16" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="H16" s="57">
+      <c r="H16" s="41">
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="49" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="43" t="s">
+    <row r="17" spans="2:8" s="35" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="44"/>
-      <c r="E17" s="45" t="s">
+      <c r="D17" s="63"/>
+      <c r="E17" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="46" t="s">
+      <c r="F17" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="G17" s="45" t="s">
+      <c r="G17" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="42">
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="2:8" s="36" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="50" t="s">
+    <row r="18" spans="2:8" s="24" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-    </row>
-    <row r="19" spans="2:8" s="36" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-    </row>
-    <row r="20" spans="2:8" s="36" customFormat="1" ht="15.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="60" t="s">
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+    </row>
+    <row r="19" spans="2:8" s="24" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+    </row>
+    <row r="20" spans="2:8" s="24" customFormat="1" ht="15.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
     </row>
     <row r="21" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
     </row>
     <row r="22" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
     </row>
     <row r="23" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="63"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
     </row>
     <row r="24" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="64"/>
-      <c r="G24" s="64"/>
-      <c r="H24" s="64"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
     </row>
     <row r="25" spans="2:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="65"/>
+      <c r="B25" s="47"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B26" s="52" t="s">
+      <c r="B26" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="66"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="52"/>
-    </row>
-    <row r="27" spans="2:8" ht="39.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="67" t="s">
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="16"/>
+    </row>
+    <row r="27" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-    </row>
-    <row r="28" spans="2:8" s="49" customFormat="1" ht="26.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="67" t="s">
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="47"/>
+    </row>
+    <row r="28" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="47"/>
+      <c r="D28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
+    </row>
+    <row r="29" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+    </row>
+    <row r="30" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+    </row>
+    <row r="31" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+    </row>
+    <row r="32" spans="2:8" s="35" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="C28" s="65"/>
-      <c r="D28" s="65"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-    </row>
-    <row r="29" spans="2:8" s="49" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="67" t="s">
+      <c r="C32" s="47"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+    </row>
+    <row r="33" spans="2:8" s="35" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="63"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="63"/>
-      <c r="H29" s="63"/>
-    </row>
-    <row r="30" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="67" t="s">
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+    </row>
+    <row r="34" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B34" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="49"/>
-      <c r="H30" s="49"/>
-    </row>
-    <row r="31" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="67" t="s">
+      <c r="C34" s="47"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+    </row>
+    <row r="35" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B35" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-    </row>
-    <row r="32" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="67" t="s">
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+    </row>
+    <row r="36" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B36" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
-    </row>
-    <row r="33" spans="2:8" s="49" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="67" t="s">
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="47"/>
+    </row>
+    <row r="37" spans="2:8" s="35" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="63"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="63"/>
-    </row>
-    <row r="34" spans="2:8" s="49" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="67" t="s">
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="47"/>
+    </row>
+    <row r="38" spans="2:8" s="35" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="63"/>
-    </row>
-    <row r="35" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="67" t="s">
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
+    </row>
+    <row r="39" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B39" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="64"/>
-    </row>
-    <row r="36" spans="2:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B37" s="52" t="s">
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B41" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="66"/>
-      <c r="D37" s="66"/>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="66"/>
-    </row>
-    <row r="38" spans="2:8" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="67" t="s">
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="48"/>
+    </row>
+    <row r="42" spans="2:8" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B42" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="65"/>
-      <c r="D38" s="65"/>
-      <c r="E38" s="65"/>
-      <c r="F38" s="65"/>
-      <c r="G38" s="65"/>
-      <c r="H38" s="65"/>
-    </row>
-    <row r="39" spans="2:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="67" t="s">
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+    </row>
+    <row r="43" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="65"/>
-      <c r="D39" s="65"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="65"/>
-      <c r="G39" s="65"/>
-      <c r="H39" s="65"/>
-    </row>
-    <row r="40" spans="2:8" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="67" t="s">
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="47"/>
+    </row>
+    <row r="44" spans="2:8" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B44" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="65"/>
-      <c r="D40" s="65"/>
-      <c r="E40" s="65"/>
-      <c r="F40" s="65"/>
-      <c r="G40" s="65"/>
-      <c r="H40" s="65"/>
-    </row>
-    <row r="41" spans="2:8" ht="53.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="67" t="s">
+      <c r="C44" s="47"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="47"/>
+    </row>
+    <row r="45" spans="2:8" ht="54.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B45" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="65"/>
-      <c r="D41" s="65"/>
-      <c r="E41" s="65"/>
-      <c r="F41" s="65"/>
-      <c r="G41" s="65"/>
-      <c r="H41" s="65"/>
-    </row>
-    <row r="42" spans="2:8" ht="84" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="67" t="s">
+      <c r="C45" s="47"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="47"/>
+      <c r="H45" s="47"/>
+    </row>
+    <row r="46" spans="2:8" ht="84" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B46" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="65"/>
-    </row>
-    <row r="43" spans="2:8" ht="12.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B44" s="52" t="s">
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="47"/>
+      <c r="G46" s="47"/>
+      <c r="H46" s="47"/>
+    </row>
+    <row r="47" spans="2:8" ht="12.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B48" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="66"/>
-      <c r="D44" s="66"/>
-      <c r="E44" s="66"/>
-      <c r="F44" s="66"/>
-      <c r="G44" s="66"/>
-      <c r="H44" s="66"/>
-    </row>
-    <row r="45" spans="2:8" s="68" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="67" t="s">
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="48"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="48"/>
+    </row>
+    <row r="49" spans="2:8" s="50" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B49" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="65"/>
-      <c r="D45" s="65"/>
-      <c r="E45" s="65"/>
-      <c r="F45" s="65"/>
-      <c r="G45" s="65"/>
-      <c r="H45" s="65"/>
-    </row>
-    <row r="46" spans="2:8" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="67" t="s">
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="47"/>
+      <c r="H49" s="47"/>
+    </row>
+    <row r="50" spans="2:8" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B50" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="63"/>
-      <c r="D46" s="63"/>
-      <c r="E46" s="63"/>
-      <c r="F46" s="63"/>
-      <c r="G46" s="63"/>
-      <c r="H46" s="63"/>
-    </row>
-    <row r="47" spans="2:8" ht="26.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="67" t="s">
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+    </row>
+    <row r="51" spans="2:8" ht="26.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B51" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="C47" s="65"/>
-      <c r="D47" s="65"/>
-      <c r="E47" s="65"/>
-      <c r="F47" s="65"/>
-      <c r="G47" s="65"/>
-      <c r="H47" s="65"/>
-    </row>
-    <row r="48" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B48" s="67" t="s">
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="47"/>
+      <c r="H51" s="47"/>
+    </row>
+    <row r="52" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B52" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="C48" s="65"/>
-      <c r="D48" s="65"/>
-      <c r="E48" s="65"/>
-      <c r="F48" s="65"/>
-      <c r="G48" s="65"/>
-      <c r="H48" s="65"/>
-    </row>
-    <row r="49" spans="2:8" ht="41.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B49" s="67" t="s">
+      <c r="C52" s="47"/>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="47"/>
+      <c r="H52" s="47"/>
+    </row>
+    <row r="53" spans="2:8" ht="41.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B53" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="C49" s="65"/>
-      <c r="D49" s="65"/>
-      <c r="E49" s="65"/>
-      <c r="F49" s="65"/>
-      <c r="G49" s="65"/>
-      <c r="H49" s="65"/>
-    </row>
-    <row r="50" spans="2:8" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="67" t="s">
+      <c r="C53" s="47"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="47"/>
+      <c r="H53" s="47"/>
+    </row>
+    <row r="54" spans="2:8" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B54" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="65"/>
-      <c r="D50" s="65"/>
-      <c r="E50" s="65"/>
-      <c r="F50" s="65"/>
-      <c r="G50" s="65"/>
-      <c r="H50" s="65"/>
-    </row>
-    <row r="51" spans="2:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B52" s="52" t="s">
+      <c r="C54" s="47"/>
+      <c r="D54" s="47"/>
+      <c r="E54" s="47"/>
+      <c r="F54" s="47"/>
+      <c r="G54" s="47"/>
+      <c r="H54" s="47"/>
+    </row>
+    <row r="55" spans="2:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B56" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C52" s="66"/>
-      <c r="D52" s="66"/>
-      <c r="E52" s="66"/>
-      <c r="F52" s="66"/>
-      <c r="G52" s="66"/>
-      <c r="H52" s="66"/>
-    </row>
-    <row r="53" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="67" t="s">
+      <c r="C56" s="48"/>
+      <c r="D56" s="48"/>
+      <c r="E56" s="48"/>
+      <c r="F56" s="48"/>
+      <c r="G56" s="48"/>
+      <c r="H56" s="48"/>
+    </row>
+    <row r="57" spans="2:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B57" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="C53" s="65"/>
-      <c r="D53" s="65"/>
-      <c r="E53" s="65"/>
-      <c r="F53" s="65"/>
-      <c r="G53" s="65"/>
-      <c r="H53" s="65"/>
-    </row>
-    <row r="54" spans="2:8" s="63" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B54" s="67" t="s">
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
+      <c r="F57" s="47"/>
+      <c r="G57" s="47"/>
+      <c r="H57" s="47"/>
+    </row>
+    <row r="58" spans="2:8" s="45" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B58" s="49" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="26.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="67" t="s">
+    <row r="59" spans="2:8" ht="26.65" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B59" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="C55" s="63"/>
-      <c r="D55" s="63"/>
-      <c r="E55" s="63"/>
-      <c r="F55" s="63"/>
-      <c r="G55" s="63"/>
-      <c r="H55" s="63"/>
-    </row>
-    <row r="56" spans="2:8" s="49" customFormat="1" ht="40.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="67" t="s">
+      <c r="C59" s="45"/>
+      <c r="D59" s="45"/>
+      <c r="E59" s="45"/>
+      <c r="F59" s="45"/>
+      <c r="G59" s="45"/>
+      <c r="H59" s="45"/>
+    </row>
+    <row r="60" spans="2:8" s="35" customFormat="1" ht="40.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B60" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="C56" s="65"/>
-      <c r="D56" s="65"/>
-      <c r="E56" s="65"/>
-      <c r="F56" s="65"/>
-      <c r="G56" s="65"/>
-      <c r="H56" s="65"/>
-    </row>
-    <row r="57" spans="2:8" s="69" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B57" s="67" t="s">
+      <c r="C60" s="47"/>
+      <c r="D60" s="47"/>
+      <c r="E60" s="47"/>
+      <c r="F60" s="47"/>
+      <c r="G60" s="47"/>
+      <c r="H60" s="47"/>
+    </row>
+    <row r="61" spans="2:8" s="51" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B61" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="C57" s="63"/>
-      <c r="D57" s="63"/>
-      <c r="E57" s="63"/>
-      <c r="F57" s="63"/>
-      <c r="G57" s="63"/>
-      <c r="H57" s="63"/>
-    </row>
-    <row r="58" spans="2:8" s="68" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B58" s="67" t="s">
+      <c r="C61" s="45"/>
+      <c r="D61" s="45"/>
+      <c r="E61" s="45"/>
+      <c r="F61" s="45"/>
+      <c r="G61" s="45"/>
+      <c r="H61" s="45"/>
+    </row>
+    <row r="62" spans="2:8" s="50" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B62" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="C58" s="65"/>
-      <c r="D58" s="65"/>
-      <c r="E58" s="65"/>
-      <c r="F58" s="65"/>
-      <c r="G58" s="65"/>
-      <c r="H58" s="65"/>
-    </row>
-    <row r="59" spans="2:8" s="49" customFormat="1" ht="44.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B59" s="67" t="s">
+      <c r="C62" s="47"/>
+      <c r="D62" s="47"/>
+      <c r="E62" s="47"/>
+      <c r="F62" s="47"/>
+      <c r="G62" s="47"/>
+      <c r="H62" s="47"/>
+    </row>
+    <row r="63" spans="2:8" s="35" customFormat="1" ht="44.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B63" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="C59" s="65"/>
-      <c r="D59" s="65"/>
-      <c r="E59" s="65"/>
-      <c r="F59" s="65"/>
-      <c r="G59" s="65"/>
-      <c r="H59" s="65"/>
-    </row>
-    <row r="60" spans="2:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="61" spans="2:8" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B61" s="70" t="s">
+      <c r="C63" s="47"/>
+      <c r="D63" s="47"/>
+      <c r="E63" s="47"/>
+      <c r="F63" s="47"/>
+      <c r="G63" s="47"/>
+      <c r="H63" s="47"/>
+    </row>
+    <row r="64" spans="2:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="65" spans="2:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B65" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="25"/>
-      <c r="H61" s="25"/>
-    </row>
-    <row r="62" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="71" t="s">
+      <c r="C65" s="17"/>
+      <c r="D65" s="17"/>
+      <c r="E65" s="17"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="17"/>
+      <c r="H65" s="17"/>
+    </row>
+    <row r="66" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B66" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="C62" s="66" t="s">
+      <c r="C66" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="D62" s="72"/>
-      <c r="F62" s="71" t="s">
+      <c r="D66" s="53"/>
+      <c r="F66" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="G62" s="66"/>
-      <c r="H62" s="66" t="s">
+      <c r="G66" s="48"/>
+      <c r="H66" s="48" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="63" spans="2:8" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B63" s="80" t="s">
+    <row r="67" spans="2:8" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B67" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="C63" s="64"/>
-      <c r="D63" s="64"/>
-      <c r="F63" s="80" t="s">
+      <c r="C67" s="46"/>
+      <c r="D67" s="46"/>
+      <c r="F67" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="G63" s="49"/>
-      <c r="H63" s="49"/>
-    </row>
-    <row r="64" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B64" s="80" t="s">
+      <c r="G67" s="35"/>
+      <c r="H67" s="35"/>
+    </row>
+    <row r="68" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B68" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="C64" s="64"/>
-      <c r="D64" s="64"/>
-      <c r="F64" s="80" t="s">
+      <c r="C68" s="46"/>
+      <c r="D68" s="46"/>
+      <c r="F68" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="G64" s="64"/>
-      <c r="H64" s="64"/>
-    </row>
-    <row r="65" spans="2:8" ht="12.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B65" s="80" t="s">
+      <c r="G68" s="46"/>
+      <c r="H68" s="46"/>
+    </row>
+    <row r="69" spans="2:8" ht="12.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B69" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="C65" s="73"/>
-      <c r="D65" s="64"/>
-      <c r="F65" s="80" t="s">
+      <c r="C69" s="78"/>
+      <c r="D69" s="46"/>
+      <c r="F69" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="G65" s="64"/>
-      <c r="H65" s="64"/>
-    </row>
-    <row r="66" spans="2:8" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B66" s="80" t="s">
+      <c r="G69" s="46"/>
+      <c r="H69" s="46"/>
+    </row>
+    <row r="70" spans="2:8" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B70" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C66" s="64"/>
-      <c r="D66" s="64"/>
-      <c r="F66" s="80" t="s">
+      <c r="C70" s="46"/>
+      <c r="D70" s="46"/>
+      <c r="F70" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="G66" s="64"/>
-      <c r="H66" s="64"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B67" s="80" t="s">
+      <c r="G70" s="46"/>
+      <c r="H70" s="46"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B71" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="C67" s="64"/>
-      <c r="D67" s="74"/>
-      <c r="F67" s="80" t="s">
+      <c r="C71" s="46"/>
+      <c r="D71" s="54"/>
+      <c r="F71" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="G67" s="64"/>
-      <c r="H67" s="64"/>
-    </row>
-    <row r="68" spans="2:8" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B68" s="80" t="s">
+      <c r="G71" s="46"/>
+      <c r="H71" s="46"/>
+    </row>
+    <row r="72" spans="2:8" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B72" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="C68" s="49"/>
-      <c r="F68" s="80" t="s">
+      <c r="C72" s="35"/>
+      <c r="F72" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="G68" s="49"/>
-      <c r="H68" s="49"/>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B69" s="80" t="s">
+      <c r="G72" s="35"/>
+      <c r="H72" s="35"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B73" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="C69" s="64"/>
-      <c r="D69" s="64"/>
-      <c r="F69" s="80" t="s">
+      <c r="C73" s="46"/>
+      <c r="D73" s="46"/>
+      <c r="F73" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="G69" s="64"/>
-      <c r="H69" s="64"/>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B70" s="80" t="s">
+      <c r="G73" s="46"/>
+      <c r="H73" s="46"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B74" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="C70" s="64"/>
-      <c r="D70" s="64"/>
-      <c r="F70" s="80" t="s">
+      <c r="C74" s="46"/>
+      <c r="D74" s="46"/>
+      <c r="F74" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="G70" s="64"/>
-      <c r="H70" s="64"/>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B71" s="80" t="s">
+      <c r="G74" s="46"/>
+      <c r="H74" s="46"/>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B75" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="C71" s="64"/>
-      <c r="D71" s="64"/>
-      <c r="F71" s="80" t="s">
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
+      <c r="F75" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="G71" s="64"/>
-      <c r="H71" s="64"/>
-    </row>
-    <row r="73" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B74" s="75" t="s">
+      <c r="G75" s="46"/>
+      <c r="H75" s="46"/>
+    </row>
+    <row r="77" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B78" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="C74" s="75"/>
-      <c r="D74" s="53"/>
-      <c r="F74" s="79" t="s">
+      <c r="C78" s="60"/>
+      <c r="D78" s="38"/>
+      <c r="F78" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="G74" s="79"/>
-      <c r="H74" s="79"/>
-    </row>
-    <row r="75" spans="2:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B75" s="76"/>
-      <c r="C75" s="77"/>
-      <c r="F75" s="78"/>
-      <c r="G75" s="78"/>
-      <c r="H75" s="78"/>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B76" s="75" t="s">
+      <c r="G78" s="59"/>
+      <c r="H78" s="59"/>
+    </row>
+    <row r="79" spans="2:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B79" s="55"/>
+      <c r="C79" s="56"/>
+      <c r="F79" s="57"/>
+      <c r="G79" s="57"/>
+      <c r="H79" s="57"/>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B80" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="C76" s="75"/>
-      <c r="D76" s="53"/>
-      <c r="F76" s="75" t="s">
+      <c r="C80" s="60"/>
+      <c r="D80" s="38"/>
+      <c r="F80" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="G76" s="75"/>
-      <c r="H76" s="75"/>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="H77" s="23" t="s">
+      <c r="G80" s="60"/>
+      <c r="H80" s="60"/>
+    </row>
+    <row r="81" spans="8:8" x14ac:dyDescent="0.4">
+      <c r="H81" s="15" t="s">
         <v>104</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="F80:H80"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B80:C80"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
@@ -2488,17 +2543,12 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="7.874015748031496E-2" right="7.874015748031496E-2" top="0.19685039370078741" bottom="0.19685039370078741" header="0.11811023622047245" footer="0"/>
-  <pageSetup paperSize="9" scale="80" fitToHeight="2" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="79" fitToHeight="2" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="40" max="8" man="1"/>
+    <brk id="44" max="8" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -2522,11 +2572,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="23.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
     </row>
     <row r="2" spans="2:4" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
@@ -2537,54 +2587,54 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="99.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
     </row>
     <row r="5" spans="2:4" ht="26.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
     </row>
     <row r="6" spans="2:4" s="7" customFormat="1" ht="35.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
     </row>
     <row r="7" spans="2:4" s="8" customFormat="1" ht="35.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
     </row>
     <row r="9" spans="2:4" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="2:4" ht="14.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B11" s="3" t="s">
@@ -2592,291 +2642,291 @@
       </c>
     </row>
     <row r="12" spans="2:4" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
     </row>
     <row r="13" spans="2:4" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
     </row>
     <row r="14" spans="2:4" s="7" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
     </row>
     <row r="16" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
     </row>
     <row r="17" spans="2:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
     </row>
     <row r="18" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="72"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
     </row>
     <row r="24" spans="2:4" ht="39.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
     </row>
     <row r="25" spans="2:4" s="8" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
     </row>
     <row r="26" spans="2:4" s="8" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="71"/>
     </row>
     <row r="27" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="72"/>
     </row>
     <row r="30" spans="2:4" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
     </row>
     <row r="31" spans="2:4" s="8" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="72"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
+      <c r="C34" s="73"/>
+      <c r="D34" s="73"/>
     </row>
     <row r="35" spans="2:4" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
     </row>
     <row r="36" spans="2:4" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="71"/>
     </row>
     <row r="37" spans="2:4" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="71"/>
     </row>
     <row r="38" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="76"/>
     </row>
     <row r="39" spans="2:4" ht="113.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="70"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73"/>
     </row>
     <row r="42" spans="2:4" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
     </row>
     <row r="43" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="71"/>
     </row>
     <row r="44" spans="2:4" ht="30.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
+      <c r="C44" s="70"/>
+      <c r="D44" s="70"/>
     </row>
     <row r="45" spans="2:4" ht="42.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="C45" s="70"/>
+      <c r="D45" s="70"/>
     </row>
     <row r="46" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
+      <c r="C46" s="70"/>
+      <c r="D46" s="70"/>
     </row>
     <row r="47" spans="2:4" ht="39" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
+      <c r="C47" s="70"/>
+      <c r="D47" s="70"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
+      <c r="C49" s="73"/>
+      <c r="D49" s="73"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B50" s="18" t="s">
+      <c r="B50" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
+      <c r="C50" s="70"/>
+      <c r="D50" s="70"/>
     </row>
     <row r="51" spans="2:4" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
+      <c r="C51" s="70"/>
+      <c r="D51" s="70"/>
     </row>
     <row r="52" spans="2:4" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="17"/>
-      <c r="D52" s="17"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="71"/>
     </row>
     <row r="53" spans="2:4" s="8" customFormat="1" ht="36.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="17"/>
-      <c r="D53" s="17"/>
+      <c r="C53" s="71"/>
+      <c r="D53" s="71"/>
     </row>
     <row r="54" spans="2:4" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B54" s="18" t="s">
+      <c r="B54" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
+      <c r="C54" s="70"/>
+      <c r="D54" s="70"/>
     </row>
     <row r="55" spans="2:4" s="5" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
+      <c r="C55" s="71"/>
+      <c r="D55" s="71"/>
     </row>
     <row r="56" spans="2:4" s="8" customFormat="1" ht="51.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="71"/>
     </row>
     <row r="58" spans="2:4" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
+      <c r="C58" s="77"/>
+      <c r="D58" s="77"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B59" s="10" t="s">
@@ -2978,11 +3028,38 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B3:D3"/>
@@ -2995,38 +3072,11 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B64" r:id="rId1" display="mailto:main@sea-wolf.ru" xr:uid="{65C32F44-9D5B-4BC8-B696-A4811EE9907B}"/>

</xml_diff>

<commit_message>
innerContract cargo condition implemented (4.2 exw tmp)
</commit_message>
<xml_diff>
--- a/templates/Inner_Contract.xlsx
+++ b/templates/Inner_Contract.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAFE533-7346-4392-9DCC-A73EA6B62E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3DE145-54EC-4FFD-8415-226E5C1AAD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-55778" yWindow="-277" windowWidth="28995" windowHeight="16394" xr2:uid="{1078D20C-27F2-4BD9-B9EF-0CD976B5C671}"/>
+    <workbookView xWindow="28702" yWindow="83" windowWidth="27076" windowHeight="16995" xr2:uid="{1078D20C-27F2-4BD9-B9EF-0CD976B5C671}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="3" r:id="rId1"/>
@@ -1263,6 +1263,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
@@ -1281,47 +1299,29 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1663,8 +1663,8 @@
   </sheetPr>
   <dimension ref="B1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="148" zoomScaleNormal="100" zoomScaleSheetLayoutView="148" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:H4"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A15" zoomScale="148" zoomScaleNormal="100" zoomScaleSheetLayoutView="148" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1687,15 +1687,15 @@
       </c>
     </row>
     <row r="2" spans="2:8" ht="23.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
     </row>
     <row r="3" spans="2:8" s="18" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="17" t="s">
@@ -1704,21 +1704,21 @@
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
-      <c r="G3" s="66" t="s">
+      <c r="G3" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="66"/>
+      <c r="H3" s="61"/>
     </row>
     <row r="4" spans="2:8" ht="66" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
     </row>
     <row r="5" spans="2:8" ht="5.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="19"/>
@@ -1730,54 +1730,54 @@
       <c r="H5" s="19"/>
     </row>
     <row r="6" spans="2:8" s="18" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
     </row>
     <row r="7" spans="2:8" ht="29.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
     </row>
     <row r="8" spans="2:8" s="24" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="61"/>
+      <c r="D8" s="67"/>
       <c r="E8" s="22" t="s">
         <v>77</v>
       </c>
       <c r="F8" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="61" t="s">
+      <c r="G8" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="64"/>
+      <c r="H8" s="70"/>
     </row>
     <row r="9" spans="2:8" s="24" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="62"/>
+      <c r="D9" s="68"/>
       <c r="E9" s="26" t="s">
         <v>80</v>
       </c>
@@ -1793,10 +1793,10 @@
       <c r="B10" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="D10" s="63"/>
+      <c r="D10" s="69"/>
       <c r="E10" s="31" t="s">
         <v>82</v>
       </c>
@@ -1842,10 +1842,10 @@
       <c r="B15" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="61" t="s">
+      <c r="C15" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="61"/>
+      <c r="D15" s="67"/>
       <c r="E15" s="22" t="s">
         <v>77</v>
       </c>
@@ -1863,10 +1863,10 @@
       <c r="B16" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="62" t="s">
+      <c r="C16" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="62"/>
+      <c r="D16" s="68"/>
       <c r="E16" s="26" t="s">
         <v>80</v>
       </c>
@@ -1884,10 +1884,10 @@
       <c r="B17" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="63" t="s">
+      <c r="C17" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="63"/>
+      <c r="D17" s="69"/>
       <c r="E17" s="31" t="s">
         <v>82</v>
       </c>
@@ -1985,7 +1985,7 @@
       <c r="H26" s="16"/>
     </row>
     <row r="27" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="49" t="s">
         <v>109</v>
       </c>
       <c r="C27" s="47"/>
@@ -1996,7 +1996,7 @@
       <c r="H27" s="47"/>
     </row>
     <row r="28" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="49" t="s">
         <v>111</v>
       </c>
       <c r="C28" s="47"/>
@@ -2006,7 +2006,7 @@
       <c r="H28" s="47"/>
     </row>
     <row r="29" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="47" t="s">
+      <c r="B29" s="49" t="s">
         <v>112</v>
       </c>
       <c r="C29" s="47"/>
@@ -2017,7 +2017,7 @@
       <c r="H29" s="47"/>
     </row>
     <row r="30" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="49" t="s">
         <v>113</v>
       </c>
       <c r="C30" s="47"/>
@@ -2028,7 +2028,7 @@
       <c r="H30" s="47"/>
     </row>
     <row r="31" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="49" t="s">
         <v>114</v>
       </c>
       <c r="C31" s="47"/>
@@ -2039,7 +2039,7 @@
       <c r="H31" s="47"/>
     </row>
     <row r="32" spans="2:8" s="35" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="47" t="s">
+      <c r="B32" s="49" t="s">
         <v>110</v>
       </c>
       <c r="C32" s="47"/>
@@ -2050,7 +2050,7 @@
       <c r="H32" s="47"/>
     </row>
     <row r="33" spans="2:8" s="35" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="47" t="s">
+      <c r="B33" s="49" t="s">
         <v>19</v>
       </c>
       <c r="C33" s="47"/>
@@ -2061,7 +2061,7 @@
       <c r="H33" s="47"/>
     </row>
     <row r="34" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="49" t="s">
         <v>20</v>
       </c>
       <c r="C34" s="47"/>
@@ -2072,7 +2072,7 @@
       <c r="H34" s="47"/>
     </row>
     <row r="35" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="49" t="s">
         <v>21</v>
       </c>
       <c r="C35" s="47"/>
@@ -2083,7 +2083,7 @@
       <c r="H35" s="47"/>
     </row>
     <row r="36" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="47" t="s">
+      <c r="B36" s="49" t="s">
         <v>22</v>
       </c>
       <c r="C36" s="47"/>
@@ -2094,7 +2094,7 @@
       <c r="H36" s="47"/>
     </row>
     <row r="37" spans="2:8" s="35" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="47" t="s">
+      <c r="B37" s="49" t="s">
         <v>23</v>
       </c>
       <c r="C37" s="47"/>
@@ -2105,7 +2105,7 @@
       <c r="H37" s="47"/>
     </row>
     <row r="38" spans="2:8" s="35" customFormat="1" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="47" t="s">
+      <c r="B38" s="49" t="s">
         <v>24</v>
       </c>
       <c r="C38" s="47"/>
@@ -2116,7 +2116,7 @@
       <c r="H38" s="47"/>
     </row>
     <row r="39" spans="2:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="47" t="s">
+      <c r="B39" s="49" t="s">
         <v>25</v>
       </c>
       <c r="C39" s="47"/>
@@ -2409,7 +2409,7 @@
       <c r="B69" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="C69" s="78"/>
+      <c r="C69" s="59"/>
       <c r="D69" s="46"/>
       <c r="F69" s="58" t="s">
         <v>94</v>
@@ -2490,16 +2490,16 @@
     </row>
     <row r="77" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="78" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B78" s="60" t="s">
+      <c r="B78" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="C78" s="60"/>
+      <c r="C78" s="66"/>
       <c r="D78" s="38"/>
-      <c r="F78" s="59" t="s">
+      <c r="F78" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="G78" s="59"/>
-      <c r="H78" s="59"/>
+      <c r="G78" s="65"/>
+      <c r="H78" s="65"/>
     </row>
     <row r="79" spans="2:8" ht="19.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B79" s="55"/>
@@ -2509,16 +2509,16 @@
       <c r="H79" s="57"/>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B80" s="60" t="s">
+      <c r="B80" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="C80" s="60"/>
+      <c r="C80" s="66"/>
       <c r="D80" s="38"/>
-      <c r="F80" s="60" t="s">
+      <c r="F80" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="G80" s="60"/>
-      <c r="H80" s="60"/>
+      <c r="G80" s="66"/>
+      <c r="H80" s="66"/>
     </row>
     <row r="81" spans="8:8" x14ac:dyDescent="0.4">
       <c r="H81" s="15" t="s">
@@ -2527,11 +2527,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B2:H2"/>
     <mergeCell ref="F78:H78"/>
     <mergeCell ref="F80:H80"/>
     <mergeCell ref="B78:C78"/>
@@ -2543,6 +2538,11 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="G8:H8"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="7.874015748031496E-2" right="7.874015748031496E-2" top="0.19685039370078741" bottom="0.19685039370078741" header="0.11811023622047245" footer="0"/>
@@ -2572,11 +2572,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="23.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
     </row>
     <row r="2" spans="2:4" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
@@ -2587,18 +2587,18 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="99.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
     </row>
     <row r="5" spans="2:4" ht="26.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="71" t="s">
@@ -2622,19 +2622,19 @@
       <c r="D7" s="71"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
     </row>
     <row r="9" spans="2:4" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="2:4" ht="14.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B11" s="3" t="s">
@@ -2663,18 +2663,18 @@
       <c r="D14" s="71"/>
     </row>
     <row r="16" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
+      <c r="C16" s="74"/>
+      <c r="D16" s="74"/>
     </row>
     <row r="17" spans="2:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="70" t="s">
+      <c r="B17" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
     </row>
     <row r="18" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="71" t="s">
@@ -2691,25 +2691,25 @@
       <c r="D19" s="71"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B20" s="72" t="s">
+      <c r="B20" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="72"/>
-      <c r="D20" s="72"/>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B21" s="72" t="s">
+      <c r="B21" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
     </row>
     <row r="24" spans="2:4" ht="39.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="71" t="s">
@@ -2740,18 +2740,18 @@
       <c r="D27" s="71"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B28" s="72" t="s">
+      <c r="B28" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
+      <c r="C28" s="76"/>
+      <c r="D28" s="76"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B29" s="72" t="s">
+      <c r="B29" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="72"/>
-      <c r="D29" s="72"/>
+      <c r="C29" s="76"/>
+      <c r="D29" s="76"/>
     </row>
     <row r="30" spans="2:4" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B30" s="71" t="s">
@@ -2768,18 +2768,18 @@
       <c r="D31" s="71"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B32" s="72" t="s">
+      <c r="B32" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="76"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B34" s="73" t="s">
+      <c r="B34" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="74"/>
     </row>
     <row r="35" spans="2:4" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B35" s="71" t="s">
@@ -2803,25 +2803,25 @@
       <c r="D37" s="71"/>
     </row>
     <row r="38" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="76" t="s">
+      <c r="B38" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="76"/>
-      <c r="D38" s="76"/>
+      <c r="C38" s="75"/>
+      <c r="D38" s="75"/>
     </row>
     <row r="39" spans="2:4" ht="113.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="70" t="s">
+      <c r="B39" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="70"/>
-      <c r="D39" s="70"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B41" s="73" t="s">
+      <c r="B41" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="73"/>
-      <c r="D41" s="73"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
     </row>
     <row r="42" spans="2:4" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B42" s="71" t="s">
@@ -2838,53 +2838,53 @@
       <c r="D43" s="71"/>
     </row>
     <row r="44" spans="2:4" ht="30.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="70" t="s">
+      <c r="B44" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="70"/>
-      <c r="D44" s="70"/>
+      <c r="C44" s="73"/>
+      <c r="D44" s="73"/>
     </row>
     <row r="45" spans="2:4" ht="42.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="70" t="s">
+      <c r="B45" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="70"/>
-      <c r="D45" s="70"/>
+      <c r="C45" s="73"/>
+      <c r="D45" s="73"/>
     </row>
     <row r="46" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="70" t="s">
+      <c r="B46" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="70"/>
-      <c r="D46" s="70"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="73"/>
     </row>
     <row r="47" spans="2:4" ht="39" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="70" t="s">
+      <c r="B47" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="70"/>
-      <c r="D47" s="70"/>
+      <c r="C47" s="73"/>
+      <c r="D47" s="73"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B49" s="73" t="s">
+      <c r="B49" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="73"/>
-      <c r="D49" s="73"/>
+      <c r="C49" s="74"/>
+      <c r="D49" s="74"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B50" s="70" t="s">
+      <c r="B50" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="70"/>
-      <c r="D50" s="70"/>
+      <c r="C50" s="73"/>
+      <c r="D50" s="73"/>
     </row>
     <row r="51" spans="2:4" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="70" t="s">
+      <c r="B51" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="70"/>
-      <c r="D51" s="70"/>
+      <c r="C51" s="73"/>
+      <c r="D51" s="73"/>
     </row>
     <row r="52" spans="2:4" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B52" s="71" t="s">
@@ -2901,11 +2901,11 @@
       <c r="D53" s="71"/>
     </row>
     <row r="54" spans="2:4" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B54" s="70" t="s">
+      <c r="B54" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="70"/>
-      <c r="D54" s="70"/>
+      <c r="C54" s="73"/>
+      <c r="D54" s="73"/>
     </row>
     <row r="55" spans="2:4" s="5" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B55" s="71" t="s">
@@ -2922,11 +2922,11 @@
       <c r="D56" s="71"/>
     </row>
     <row r="58" spans="2:4" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="77" t="s">
+      <c r="B58" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="77"/>
-      <c r="D58" s="77"/>
+      <c r="C58" s="72"/>
+      <c r="D58" s="72"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B59" s="10" t="s">
@@ -3028,38 +3028,11 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B3:D3"/>
@@ -3072,11 +3045,38 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B64" r:id="rId1" display="mailto:main@sea-wolf.ru" xr:uid="{65C32F44-9D5B-4BC8-B696-A4811EE9907B}"/>

</xml_diff>

<commit_message>
innercontract tmp merge cells bug fixed
</commit_message>
<xml_diff>
--- a/templates/Inner_Contract.xlsx
+++ b/templates/Inner_Contract.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6C6DE7-228F-4560-A5E7-DF0798967C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A66B01-CFC5-4FA2-B1C7-9B14D97EFF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{1078D20C-27F2-4BD9-B9EF-0CD976B5C671}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{1078D20C-27F2-4BD9-B9EF-0CD976B5C671}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="3" r:id="rId1"/>
@@ -1024,7 +1024,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1205,17 +1205,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
@@ -1233,31 +1224,28 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1599,8 +1587,8 @@
   </sheetPr>
   <dimension ref="B1:H98"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A63" zoomScale="96" zoomScaleNormal="100" zoomScaleSheetLayoutView="96" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="96" zoomScaleNormal="100" zoomScaleSheetLayoutView="96" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1623,15 +1611,15 @@
       </c>
     </row>
     <row r="2" spans="2:8" ht="23.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
     </row>
     <row r="3" spans="2:8" s="18" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="17" t="s">
@@ -1640,21 +1628,21 @@
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
-      <c r="G3" s="69" t="s">
+      <c r="G3" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="69"/>
+      <c r="H3" s="66"/>
     </row>
     <row r="4" spans="2:8" ht="71.349999999999994" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
     </row>
     <row r="5" spans="2:8" ht="5.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="19"/>
@@ -1666,35 +1654,35 @@
       <c r="H5" s="19"/>
     </row>
     <row r="6" spans="2:8" s="18" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
     </row>
     <row r="7" spans="2:8" ht="29.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
     </row>
     <row r="8" spans="2:8" s="24" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="65"/>
+      <c r="D8" s="61"/>
       <c r="E8" s="22" t="s">
         <v>77</v>
       </c>
@@ -1704,16 +1692,16 @@
       <c r="G8" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="81"/>
+      <c r="H8" s="64"/>
     </row>
     <row r="9" spans="2:8" s="24" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="66"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="26" t="s">
         <v>80</v>
       </c>
@@ -1729,10 +1717,10 @@
       <c r="B10" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="67" t="s">
+      <c r="C10" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="D10" s="67"/>
+      <c r="D10" s="33"/>
       <c r="E10" s="31" t="s">
         <v>82</v>
       </c>
@@ -1781,10 +1769,10 @@
       <c r="B15" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="61" t="s">
+      <c r="C15" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="61"/>
+      <c r="D15" s="22"/>
       <c r="E15" s="22" t="s">
         <v>77</v>
       </c>
@@ -2448,10 +2436,10 @@
       <c r="H79" s="57"/>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B80" s="64" t="s">
+      <c r="B80" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="C80" s="64"/>
+      <c r="C80" s="62"/>
       <c r="D80" s="38"/>
       <c r="F80" s="62" t="s">
         <v>75</v>
@@ -2482,16 +2470,12 @@
     <row r="97" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="98" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="5">
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="B6:H6"/>
     <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="7.874015748031496E-2" right="7.874015748031496E-2" top="0.19685039370078741" bottom="0.19685039370078741" header="0.11811023622047245" footer="0"/>
@@ -2521,11 +2505,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="23.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
     </row>
     <row r="2" spans="2:4" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
@@ -2536,39 +2520,39 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="99.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
     </row>
     <row r="5" spans="2:4" ht="26.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
     </row>
     <row r="6" spans="2:4" s="7" customFormat="1" ht="35.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
     </row>
     <row r="7" spans="2:4" s="8" customFormat="1" ht="35.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B8" s="75" t="s">
@@ -2579,11 +2563,11 @@
     </row>
     <row r="9" spans="2:4" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="2:4" ht="14.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="78" t="s">
+      <c r="B10" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B11" s="3" t="s">
@@ -2591,53 +2575,53 @@
       </c>
     </row>
     <row r="12" spans="2:4" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="70" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
     </row>
     <row r="13" spans="2:4" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="74" t="s">
+      <c r="B13" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
     </row>
     <row r="14" spans="2:4" s="7" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="74" t="s">
+      <c r="B14" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
     </row>
     <row r="16" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="76" t="s">
+      <c r="B16" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="76"/>
-      <c r="D16" s="76"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
     </row>
     <row r="17" spans="2:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
     </row>
     <row r="18" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="74" t="s">
+      <c r="B18" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="74"/>
-      <c r="D19" s="74"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B20" s="75" t="s">
@@ -2654,39 +2638,39 @@
       <c r="D21" s="75"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
     </row>
     <row r="24" spans="2:4" ht="39.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="74" t="s">
+      <c r="B24" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
     </row>
     <row r="25" spans="2:4" s="8" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="74" t="s">
+      <c r="B25" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="70"/>
     </row>
     <row r="26" spans="2:4" s="8" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="74" t="s">
+      <c r="B26" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="74"/>
-      <c r="D26" s="74"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
     </row>
     <row r="27" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="74" t="s">
+      <c r="B27" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="70"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B28" s="75" t="s">
@@ -2703,18 +2687,18 @@
       <c r="D29" s="75"/>
     </row>
     <row r="30" spans="2:4" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="74" t="s">
+      <c r="B30" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
+      <c r="C30" s="70"/>
+      <c r="D30" s="70"/>
     </row>
     <row r="31" spans="2:4" s="8" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="74" t="s">
+      <c r="B31" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="74"/>
-      <c r="D31" s="74"/>
+      <c r="C31" s="70"/>
+      <c r="D31" s="70"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B32" s="75" t="s">
@@ -2724,158 +2708,158 @@
       <c r="D32" s="75"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B34" s="76" t="s">
+      <c r="B34" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="76"/>
-      <c r="D34" s="76"/>
+      <c r="C34" s="73"/>
+      <c r="D34" s="73"/>
     </row>
     <row r="35" spans="2:4" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="74" t="s">
+      <c r="B35" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="74"/>
-      <c r="D35" s="74"/>
+      <c r="C35" s="70"/>
+      <c r="D35" s="70"/>
     </row>
     <row r="36" spans="2:4" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="74" t="s">
+      <c r="B36" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="74"/>
-      <c r="D36" s="74"/>
+      <c r="C36" s="70"/>
+      <c r="D36" s="70"/>
     </row>
     <row r="37" spans="2:4" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="74" t="s">
+      <c r="B37" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="74"/>
-      <c r="D37" s="74"/>
+      <c r="C37" s="70"/>
+      <c r="D37" s="70"/>
     </row>
     <row r="38" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="79" t="s">
+      <c r="B38" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="79"/>
-      <c r="D38" s="79"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="74"/>
     </row>
     <row r="39" spans="2:4" ht="113.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="73" t="s">
+      <c r="B39" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
+      <c r="C39" s="72"/>
+      <c r="D39" s="72"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B41" s="76" t="s">
+      <c r="B41" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="76"/>
-      <c r="D41" s="76"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73"/>
     </row>
     <row r="42" spans="2:4" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="74" t="s">
+      <c r="B42" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="74"/>
-      <c r="D42" s="74"/>
+      <c r="C42" s="70"/>
+      <c r="D42" s="70"/>
     </row>
     <row r="43" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="74" t="s">
+      <c r="B43" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="74"/>
-      <c r="D43" s="74"/>
+      <c r="C43" s="70"/>
+      <c r="D43" s="70"/>
     </row>
     <row r="44" spans="2:4" ht="30.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="73" t="s">
+      <c r="B44" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="73"/>
-      <c r="D44" s="73"/>
+      <c r="C44" s="72"/>
+      <c r="D44" s="72"/>
     </row>
     <row r="45" spans="2:4" ht="42.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="73" t="s">
+      <c r="B45" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="73"/>
-      <c r="D45" s="73"/>
+      <c r="C45" s="72"/>
+      <c r="D45" s="72"/>
     </row>
     <row r="46" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="73" t="s">
+      <c r="B46" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="73"/>
-      <c r="D46" s="73"/>
+      <c r="C46" s="72"/>
+      <c r="D46" s="72"/>
     </row>
     <row r="47" spans="2:4" ht="39" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="73" t="s">
+      <c r="B47" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="73"/>
-      <c r="D47" s="73"/>
+      <c r="C47" s="72"/>
+      <c r="D47" s="72"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B49" s="76" t="s">
+      <c r="B49" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="76"/>
-      <c r="D49" s="76"/>
+      <c r="C49" s="73"/>
+      <c r="D49" s="73"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B50" s="73" t="s">
+      <c r="B50" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="73"/>
-      <c r="D50" s="73"/>
+      <c r="C50" s="72"/>
+      <c r="D50" s="72"/>
     </row>
     <row r="51" spans="2:4" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="73" t="s">
+      <c r="B51" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="73"/>
-      <c r="D51" s="73"/>
+      <c r="C51" s="72"/>
+      <c r="D51" s="72"/>
     </row>
     <row r="52" spans="2:4" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="74" t="s">
+      <c r="B52" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="74"/>
-      <c r="D52" s="74"/>
+      <c r="C52" s="70"/>
+      <c r="D52" s="70"/>
     </row>
     <row r="53" spans="2:4" s="8" customFormat="1" ht="36.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="74" t="s">
+      <c r="B53" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="74"/>
-      <c r="D53" s="74"/>
+      <c r="C53" s="70"/>
+      <c r="D53" s="70"/>
     </row>
     <row r="54" spans="2:4" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B54" s="73" t="s">
+      <c r="B54" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="73"/>
-      <c r="D54" s="73"/>
+      <c r="C54" s="72"/>
+      <c r="D54" s="72"/>
     </row>
     <row r="55" spans="2:4" s="5" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="74" t="s">
+      <c r="B55" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="74"/>
-      <c r="D55" s="74"/>
+      <c r="C55" s="70"/>
+      <c r="D55" s="70"/>
     </row>
     <row r="56" spans="2:4" s="8" customFormat="1" ht="51.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="74" t="s">
+      <c r="B56" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="74"/>
-      <c r="D56" s="74"/>
+      <c r="C56" s="70"/>
+      <c r="D56" s="70"/>
     </row>
     <row r="58" spans="2:4" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="80" t="s">
+      <c r="B58" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="80"/>
-      <c r="D58" s="80"/>
+      <c r="C58" s="71"/>
+      <c r="D58" s="71"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B59" s="10" t="s">
@@ -2977,38 +2961,11 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B3:D3"/>
@@ -3021,11 +2978,38 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B64" r:id="rId1" display="mailto:main@sea-wolf.ru" xr:uid="{65C32F44-9D5B-4BC8-B696-A4811EE9907B}"/>

</xml_diff>

<commit_message>
port letter samples work started
</commit_message>
<xml_diff>
--- a/templates/Inner_Contract.xlsx
+++ b/templates/Inner_Contract.xlsx
@@ -1,53 +1,53 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A66B01-CFC5-4FA2-B1C7-9B14D97EFF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D98FEB6-5F7A-40D0-880E-E6B64F067961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{1078D20C-27F2-4BD9-B9EF-0CD976B5C671}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{1078D20C-27F2-4BD9-B9EF-0CD976B5C671}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Pg_end">Contract!$H$81</definedName>
+    <definedName name="Pg_end">Contract!$I$81</definedName>
     <definedName name="Pg_start">Contract!$B$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Contract!$A$2:$I$98</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Contract!$A$2:$J$99</definedName>
     <definedName name="Договор_адреса_заголовок">Contract!$B$65</definedName>
-    <definedName name="Договор_адреса_покупатель">Contract!$F$66</definedName>
-    <definedName name="Договор_адреса_покупатель_адрес">Contract!$F$67</definedName>
-    <definedName name="Договор_адреса_покупатель_банк">Contract!$F$72</definedName>
-    <definedName name="Договор_адреса_покупатель_бик">Contract!$F$73</definedName>
-    <definedName name="Договор_адреса_покупатель_должность">Contract!$F$78</definedName>
-    <definedName name="Договор_адреса_покупатель_инн">Contract!$F$70</definedName>
-    <definedName name="Договор_адреса_покупатель_конец">Contract!$H$66</definedName>
-    <definedName name="Договор_адреса_покупатель_кс">Contract!$F$74</definedName>
-    <definedName name="Договор_адреса_покупатель_огрн">Contract!$F$71</definedName>
-    <definedName name="Договор_адреса_покупатель_почта">Contract!$F$69</definedName>
-    <definedName name="Договор_адреса_покупатель_рс">Contract!$F$75</definedName>
-    <definedName name="Договор_адреса_покупатель_тел">Contract!$F$68</definedName>
-    <definedName name="Договор_адреса_покупатель_фио">Contract!$F$80</definedName>
+    <definedName name="Договор_адреса_покупатель">Contract!$G$66</definedName>
+    <definedName name="Договор_адреса_покупатель_адрес">Contract!$G$67</definedName>
+    <definedName name="Договор_адреса_покупатель_банк">Contract!$G$72</definedName>
+    <definedName name="Договор_адреса_покупатель_бик">Contract!$G$73</definedName>
+    <definedName name="Договор_адреса_покупатель_должность">Contract!$G$78</definedName>
+    <definedName name="Договор_адреса_покупатель_инн">Contract!$G$70</definedName>
+    <definedName name="Договор_адреса_покупатель_конец">Contract!$I$66</definedName>
+    <definedName name="Договор_адреса_покупатель_кс">Contract!$G$74</definedName>
+    <definedName name="Договор_адреса_покупатель_огрн">Contract!$G$71</definedName>
+    <definedName name="Договор_адреса_покупатель_почта">Contract!$G$69</definedName>
+    <definedName name="Договор_адреса_покупатель_рс">Contract!$G$75</definedName>
+    <definedName name="Договор_адреса_покупатель_тел">Contract!$G$68</definedName>
+    <definedName name="Договор_адреса_покупатель_фио">Contract!$G$80</definedName>
     <definedName name="Договор_адреса_поставщик">Contract!$B$66</definedName>
     <definedName name="Договор_адреса_поставщик_адрес">Contract!$B$67</definedName>
     <definedName name="Договор_адреса_поставщик_банк">Contract!$B$72</definedName>
     <definedName name="Договор_адреса_поставщик_бик">Contract!$B$73</definedName>
     <definedName name="Договор_адреса_поставщик_должность">Contract!$B$78</definedName>
     <definedName name="Договор_адреса_поставщик_инн">Contract!$B$70</definedName>
-    <definedName name="Договор_адреса_поставщик_конец">Contract!$C$66</definedName>
+    <definedName name="Договор_адреса_поставщик_конец">Contract!$D$66</definedName>
     <definedName name="Договор_адреса_поставщик_кс">Contract!$B$74</definedName>
     <definedName name="Договор_адреса_поставщик_огрн">Contract!$B$71</definedName>
     <definedName name="Договор_адреса_поставщик_почта">Contract!$B$69</definedName>
     <definedName name="Договор_адреса_поставщик_рс">Contract!$B$75</definedName>
     <definedName name="Договор_адреса_поставщик_тел">Contract!$B$68</definedName>
     <definedName name="Договор_адреса_поставщик_фио">Contract!$B$80</definedName>
-    <definedName name="Договор_дата">Contract!$G$3</definedName>
+    <definedName name="Договор_дата">Contract!$H$3</definedName>
     <definedName name="Договор_доставка">Contract!$B$33</definedName>
     <definedName name="Договор_качество_конец">Contract!#REF!</definedName>
     <definedName name="Договор_качество_начало">Contract!#REF!</definedName>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="110">
   <si>
     <t>ДОГОВОР ПОСТАВКИ № 551</t>
   </si>
@@ -1224,28 +1224,28 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1263,6 +1263,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>401834</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>324246</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>32741</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>62705</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="A close-up of a signature&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9D29EF8-0F85-47D4-9E1C-18DDDED87D15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="515936" y="19478426"/>
+          <a:ext cx="1595438" cy="561975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>745330</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>104180</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>376237</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>828476</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="A blue circle with two dolphins in it&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ED108FC-6E65-40A9-BFAF-5FF7FCEA6291}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="859432" y="19258360"/>
+          <a:ext cx="1595438" cy="1547812"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1585,32 +1678,33 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H98"/>
+  <dimension ref="B1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="96" zoomScaleNormal="100" zoomScaleSheetLayoutView="96" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A73" zoomScale="96" zoomScaleNormal="100" zoomScaleSheetLayoutView="96" workbookViewId="0">
+      <selection activeCell="H99" sqref="H99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="1.59765625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="39" style="15" customWidth="1"/>
-    <col min="3" max="3" width="15" style="15" customWidth="1"/>
-    <col min="4" max="4" width="10.265625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="6.59765625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="32.59765625" style="15" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="15" customWidth="1"/>
-    <col min="9" max="9" width="2.06640625" style="15" customWidth="1"/>
-    <col min="10" max="16384" width="9.06640625" style="15"/>
+    <col min="2" max="2" width="27.53125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="12.19921875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="15" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.265625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="6.59765625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="32.59765625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="15" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" style="15" customWidth="1"/>
+    <col min="10" max="10" width="2.06640625" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="9.06640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B1" s="15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="2:8" ht="23.35" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:9" ht="23.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="67" t="s">
         <v>0</v>
       </c>
@@ -1620,20 +1714,22 @@
       <c r="F2" s="67"/>
       <c r="G2" s="67"/>
       <c r="H2" s="67"/>
-    </row>
-    <row r="3" spans="2:8" s="18" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="I2" s="67"/>
+    </row>
+    <row r="3" spans="2:9" s="18" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
-      <c r="G3" s="66" t="s">
+      <c r="F3" s="17"/>
+      <c r="H3" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="66"/>
-    </row>
-    <row r="4" spans="2:8" ht="71.349999999999994" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I3" s="66"/>
+    </row>
+    <row r="4" spans="2:9" ht="71.349999999999994" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="65" t="s">
         <v>107</v>
       </c>
@@ -1643,8 +1739,9 @@
       <c r="F4" s="65"/>
       <c r="G4" s="65"/>
       <c r="H4" s="65"/>
-    </row>
-    <row r="5" spans="2:8" ht="5.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I4" s="65"/>
+    </row>
+    <row r="5" spans="2:9" ht="5.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -1652,8 +1749,9 @@
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
-    </row>
-    <row r="6" spans="2:8" s="18" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="2:9" s="18" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="68" t="s">
         <v>4</v>
       </c>
@@ -1663,8 +1761,9 @@
       <c r="F6" s="68"/>
       <c r="G6" s="68"/>
       <c r="H6" s="68"/>
-    </row>
-    <row r="7" spans="2:8" ht="29.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I6" s="68"/>
+    </row>
+    <row r="7" spans="2:9" ht="29.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="69" t="s">
         <v>5</v>
       </c>
@@ -1674,65 +1773,69 @@
       <c r="F7" s="69"/>
       <c r="G7" s="69"/>
       <c r="H7" s="69"/>
-    </row>
-    <row r="8" spans="2:8" s="24" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I7" s="69"/>
+    </row>
+    <row r="8" spans="2:9" s="24" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="22"/>
+      <c r="D8" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="61"/>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="61"/>
+      <c r="F8" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="G8" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="61" t="s">
+      <c r="H8" s="61" t="s">
         <v>90</v>
       </c>
-      <c r="H8" s="64"/>
-    </row>
-    <row r="9" spans="2:8" s="24" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I8" s="64"/>
+    </row>
+    <row r="9" spans="2:9" s="24" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="28"/>
+      <c r="F9" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="G9" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="H9" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="H9" s="29"/>
-    </row>
-    <row r="10" spans="2:8" s="35" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I9" s="29"/>
+    </row>
+    <row r="10" spans="2:9" s="35" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="31"/>
+      <c r="D10" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="33"/>
+      <c r="F10" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="G10" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="33" t="s">
+      <c r="H10" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="H10" s="34"/>
-    </row>
-    <row r="11" spans="2:8" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I10" s="34"/>
+    </row>
+    <row r="11" spans="2:9" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="60" t="s">
         <v>6</v>
       </c>
@@ -1742,93 +1845,100 @@
       <c r="F11" s="60"/>
       <c r="G11" s="60"/>
       <c r="H11" s="60"/>
-    </row>
-    <row r="12" spans="2:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I11" s="60"/>
+    </row>
+    <row r="12" spans="2:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="37"/>
-    </row>
-    <row r="13" spans="2:8" ht="14.65" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C12" s="37"/>
+    </row>
+    <row r="13" spans="2:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="38"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="38"/>
       <c r="E13" s="38"/>
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
       <c r="H13" s="38"/>
-    </row>
-    <row r="14" spans="2:8" ht="22.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I13" s="38"/>
+    </row>
+    <row r="14" spans="2:9" ht="22.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="39"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="39"/>
-      <c r="E14" s="40"/>
-    </row>
-    <row r="15" spans="2:8" s="35" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E14" s="39"/>
+      <c r="F14" s="40"/>
+    </row>
+    <row r="15" spans="2:9" s="35" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="22"/>
+      <c r="D15" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="22"/>
+      <c r="F15" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="G15" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="H15" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="H15" s="23" t="s">
+      <c r="I15" s="23" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="2:8" s="35" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:9" s="35" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="28"/>
+      <c r="F16" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="G16" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="H16" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="H16" s="41">
+      <c r="I16" s="41">
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="35" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:9" s="35" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="33" t="s">
+      <c r="C17" s="31"/>
+      <c r="D17" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="33"/>
+      <c r="F17" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="F17" s="32" t="s">
+      <c r="G17" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="H17" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="H17" s="42">
+      <c r="I17" s="42">
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="2:8" s="24" customFormat="1" ht="36.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:9" s="24" customFormat="1" ht="36.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="36" t="s">
         <v>108</v>
       </c>
@@ -1838,8 +1948,9 @@
       <c r="F18" s="36"/>
       <c r="G18" s="36"/>
       <c r="H18" s="36"/>
-    </row>
-    <row r="19" spans="2:8" s="24" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I18" s="36"/>
+    </row>
+    <row r="19" spans="2:9" s="24" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="35"/>
       <c r="C19" s="35"/>
       <c r="D19" s="35"/>
@@ -1847,642 +1958,702 @@
       <c r="F19" s="35"/>
       <c r="G19" s="35"/>
       <c r="H19" s="35"/>
-    </row>
-    <row r="20" spans="2:8" s="24" customFormat="1" ht="15.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I19" s="35"/>
+    </row>
+    <row r="20" spans="2:9" s="24" customFormat="1" ht="15.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="44"/>
+      <c r="C20" s="43"/>
       <c r="D20" s="44"/>
       <c r="E20" s="44"/>
       <c r="F20" s="44"/>
       <c r="G20" s="44"/>
       <c r="H20" s="44"/>
-    </row>
-    <row r="21" spans="2:8" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I20" s="44"/>
+    </row>
+    <row r="21" spans="2:9" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="37" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C21" s="37"/>
+    </row>
+    <row r="22" spans="2:9" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="45"/>
+      <c r="C22" s="37"/>
       <c r="D22" s="45"/>
       <c r="E22" s="45"/>
       <c r="F22" s="45"/>
       <c r="G22" s="45"/>
       <c r="H22" s="45"/>
-    </row>
-    <row r="23" spans="2:8" ht="16.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I22" s="45"/>
+    </row>
+    <row r="23" spans="2:9" ht="16.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="45"/>
+      <c r="C23" s="37"/>
       <c r="D23" s="45"/>
       <c r="E23" s="45"/>
       <c r="F23" s="45"/>
       <c r="G23" s="45"/>
       <c r="H23" s="45"/>
-    </row>
-    <row r="24" spans="2:8" ht="16.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I23" s="45"/>
+    </row>
+    <row r="24" spans="2:9" ht="16.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="46"/>
+      <c r="C24" s="37"/>
       <c r="D24" s="46"/>
       <c r="E24" s="46"/>
       <c r="F24" s="46"/>
       <c r="G24" s="46"/>
       <c r="H24" s="46"/>
-    </row>
-    <row r="25" spans="2:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I24" s="46"/>
+    </row>
+    <row r="25" spans="2:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B25" s="47"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="C25" s="47"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B26" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="48"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="48"/>
       <c r="E26" s="48"/>
       <c r="F26" s="48"/>
       <c r="G26" s="48"/>
-      <c r="H26" s="16"/>
-    </row>
-    <row r="27" spans="2:8" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H26" s="48"/>
+      <c r="I26" s="16"/>
+    </row>
+    <row r="27" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B27" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="47"/>
+      <c r="C27" s="49"/>
       <c r="D27" s="47"/>
       <c r="E27" s="47"/>
       <c r="F27" s="47"/>
       <c r="G27" s="47"/>
       <c r="H27" s="47"/>
-    </row>
-    <row r="28" spans="2:8" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I27" s="47"/>
+    </row>
+    <row r="28" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="47"/>
+      <c r="C28" s="49"/>
       <c r="D28" s="47"/>
-      <c r="F28" s="47"/>
+      <c r="E28" s="47"/>
       <c r="G28" s="47"/>
       <c r="H28" s="47"/>
-    </row>
-    <row r="29" spans="2:8" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I28" s="47"/>
+    </row>
+    <row r="29" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B29" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C29" s="47"/>
+      <c r="C29" s="49"/>
       <c r="D29" s="47"/>
       <c r="E29" s="47"/>
       <c r="F29" s="47"/>
       <c r="G29" s="47"/>
       <c r="H29" s="47"/>
-    </row>
-    <row r="30" spans="2:8" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I29" s="47"/>
+    </row>
+    <row r="30" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B30" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="47"/>
+      <c r="C30" s="49"/>
       <c r="D30" s="47"/>
       <c r="E30" s="47"/>
       <c r="F30" s="47"/>
       <c r="G30" s="47"/>
       <c r="H30" s="47"/>
-    </row>
-    <row r="31" spans="2:8" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I30" s="47"/>
+    </row>
+    <row r="31" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B31" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="47"/>
+      <c r="C31" s="49"/>
       <c r="D31" s="47"/>
       <c r="E31" s="47"/>
       <c r="F31" s="47"/>
       <c r="G31" s="47"/>
       <c r="H31" s="47"/>
-    </row>
-    <row r="32" spans="2:8" s="35" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I31" s="47"/>
+    </row>
+    <row r="32" spans="2:9" s="35" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B32" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C32" s="47"/>
+      <c r="C32" s="49"/>
       <c r="D32" s="47"/>
       <c r="E32" s="47"/>
       <c r="F32" s="47"/>
       <c r="G32" s="47"/>
       <c r="H32" s="47"/>
-    </row>
-    <row r="33" spans="2:8" s="35" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I32" s="47"/>
+    </row>
+    <row r="33" spans="2:9" s="35" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B33" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="47"/>
+      <c r="C33" s="49"/>
       <c r="D33" s="47"/>
       <c r="E33" s="47"/>
       <c r="F33" s="47"/>
       <c r="G33" s="47"/>
       <c r="H33" s="47"/>
-    </row>
-    <row r="34" spans="2:8" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I33" s="47"/>
+    </row>
+    <row r="34" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B34" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C34" s="47"/>
+      <c r="C34" s="49"/>
       <c r="D34" s="47"/>
       <c r="E34" s="47"/>
       <c r="F34" s="47"/>
       <c r="G34" s="47"/>
       <c r="H34" s="47"/>
-    </row>
-    <row r="35" spans="2:8" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I34" s="47"/>
+    </row>
+    <row r="35" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B35" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C35" s="47"/>
+      <c r="C35" s="49"/>
       <c r="D35" s="47"/>
       <c r="E35" s="47"/>
       <c r="F35" s="47"/>
       <c r="G35" s="47"/>
       <c r="H35" s="47"/>
-    </row>
-    <row r="36" spans="2:8" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I35" s="47"/>
+    </row>
+    <row r="36" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B36" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="47"/>
+      <c r="C36" s="49"/>
       <c r="D36" s="47"/>
       <c r="E36" s="47"/>
       <c r="F36" s="47"/>
       <c r="G36" s="47"/>
       <c r="H36" s="47"/>
-    </row>
-    <row r="37" spans="2:8" s="35" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I36" s="47"/>
+    </row>
+    <row r="37" spans="2:9" s="35" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B37" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C37" s="47"/>
+      <c r="C37" s="49"/>
       <c r="D37" s="47"/>
       <c r="E37" s="47"/>
       <c r="F37" s="47"/>
       <c r="G37" s="47"/>
       <c r="H37" s="47"/>
-    </row>
-    <row r="38" spans="2:8" s="35" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I37" s="47"/>
+    </row>
+    <row r="38" spans="2:9" s="35" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B38" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C38" s="47"/>
+      <c r="C38" s="49"/>
       <c r="D38" s="47"/>
       <c r="E38" s="47"/>
       <c r="F38" s="47"/>
       <c r="G38" s="47"/>
       <c r="H38" s="47"/>
-    </row>
-    <row r="39" spans="2:8" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I38" s="47"/>
+    </row>
+    <row r="39" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B39" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="47"/>
+      <c r="C39" s="49"/>
       <c r="D39" s="47"/>
       <c r="E39" s="47"/>
       <c r="F39" s="47"/>
       <c r="G39" s="47"/>
       <c r="H39" s="47"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="I39" s="47"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B41" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="48"/>
+      <c r="C41" s="16"/>
       <c r="D41" s="48"/>
       <c r="E41" s="48"/>
       <c r="F41" s="48"/>
       <c r="G41" s="48"/>
       <c r="H41" s="48"/>
-    </row>
-    <row r="42" spans="2:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I41" s="48"/>
+    </row>
+    <row r="42" spans="2:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B42" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C42" s="47"/>
+      <c r="C42" s="49"/>
       <c r="D42" s="47"/>
       <c r="E42" s="47"/>
       <c r="F42" s="47"/>
       <c r="G42" s="47"/>
       <c r="H42" s="47"/>
-    </row>
-    <row r="43" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I42" s="47"/>
+    </row>
+    <row r="43" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B43" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="47"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="47"/>
       <c r="E43" s="47"/>
       <c r="F43" s="47"/>
       <c r="G43" s="47"/>
       <c r="H43" s="47"/>
-    </row>
-    <row r="44" spans="2:8" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I43" s="47"/>
+    </row>
+    <row r="44" spans="2:9" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B44" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C44" s="47"/>
+      <c r="C44" s="49"/>
       <c r="D44" s="47"/>
       <c r="E44" s="47"/>
       <c r="F44" s="47"/>
       <c r="G44" s="47"/>
       <c r="H44" s="47"/>
-    </row>
-    <row r="45" spans="2:8" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I44" s="47"/>
+    </row>
+    <row r="45" spans="2:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B45" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="47"/>
+      <c r="C45" s="49"/>
       <c r="D45" s="47"/>
       <c r="E45" s="47"/>
       <c r="F45" s="47"/>
       <c r="G45" s="47"/>
       <c r="H45" s="47"/>
-    </row>
-    <row r="46" spans="2:8" ht="86.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I45" s="47"/>
+    </row>
+    <row r="46" spans="2:9" ht="86.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B46" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C46" s="47"/>
+      <c r="C46" s="49"/>
       <c r="D46" s="47"/>
       <c r="E46" s="47"/>
       <c r="F46" s="47"/>
       <c r="G46" s="47"/>
       <c r="H46" s="47"/>
-    </row>
-    <row r="47" spans="2:8" ht="12.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="I46" s="47"/>
+    </row>
+    <row r="47" spans="2:9" ht="12.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B48" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C48" s="48"/>
+      <c r="C48" s="16"/>
       <c r="D48" s="48"/>
       <c r="E48" s="48"/>
       <c r="F48" s="48"/>
       <c r="G48" s="48"/>
       <c r="H48" s="48"/>
-    </row>
-    <row r="49" spans="2:8" s="50" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I48" s="48"/>
+    </row>
+    <row r="49" spans="2:9" s="50" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B49" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="47"/>
+      <c r="C49" s="49"/>
       <c r="D49" s="47"/>
       <c r="E49" s="47"/>
       <c r="F49" s="47"/>
       <c r="G49" s="47"/>
       <c r="H49" s="47"/>
-    </row>
-    <row r="50" spans="2:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I49" s="47"/>
+    </row>
+    <row r="50" spans="2:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B50" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="45"/>
+      <c r="C50" s="49"/>
       <c r="D50" s="45"/>
       <c r="E50" s="45"/>
       <c r="F50" s="45"/>
       <c r="G50" s="45"/>
       <c r="H50" s="45"/>
-    </row>
-    <row r="51" spans="2:8" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I50" s="45"/>
+    </row>
+    <row r="51" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B51" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="C51" s="47"/>
+      <c r="C51" s="49"/>
       <c r="D51" s="47"/>
       <c r="E51" s="47"/>
       <c r="F51" s="47"/>
       <c r="G51" s="47"/>
       <c r="H51" s="47"/>
-    </row>
-    <row r="52" spans="2:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I51" s="47"/>
+    </row>
+    <row r="52" spans="2:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B52" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="C52" s="47"/>
+      <c r="C52" s="49"/>
       <c r="D52" s="47"/>
       <c r="E52" s="47"/>
       <c r="F52" s="47"/>
       <c r="G52" s="47"/>
       <c r="H52" s="47"/>
-    </row>
-    <row r="53" spans="2:8" ht="41.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I52" s="47"/>
+    </row>
+    <row r="53" spans="2:9" ht="41.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B53" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="C53" s="47"/>
+      <c r="C53" s="49"/>
       <c r="D53" s="47"/>
       <c r="E53" s="47"/>
       <c r="F53" s="47"/>
       <c r="G53" s="47"/>
       <c r="H53" s="47"/>
-    </row>
-    <row r="54" spans="2:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I53" s="47"/>
+    </row>
+    <row r="54" spans="2:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B54" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="C54" s="47"/>
+      <c r="C54" s="49"/>
       <c r="D54" s="47"/>
       <c r="E54" s="47"/>
       <c r="F54" s="47"/>
       <c r="G54" s="47"/>
       <c r="H54" s="47"/>
-    </row>
-    <row r="55" spans="2:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="I54" s="47"/>
+    </row>
+    <row r="55" spans="2:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B56" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C56" s="48"/>
+      <c r="C56" s="16"/>
       <c r="D56" s="48"/>
       <c r="E56" s="48"/>
       <c r="F56" s="48"/>
       <c r="G56" s="48"/>
       <c r="H56" s="48"/>
-    </row>
-    <row r="57" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I56" s="48"/>
+    </row>
+    <row r="57" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B57" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="C57" s="47"/>
+      <c r="C57" s="49"/>
       <c r="D57" s="47"/>
       <c r="E57" s="47"/>
       <c r="F57" s="47"/>
       <c r="G57" s="47"/>
       <c r="H57" s="47"/>
-    </row>
-    <row r="58" spans="2:8" s="45" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="I57" s="47"/>
+    </row>
+    <row r="58" spans="2:9" s="45" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B58" s="49" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="59" spans="2:8" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C58" s="49"/>
+    </row>
+    <row r="59" spans="2:9" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B59" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="C59" s="45"/>
+      <c r="C59" s="49"/>
       <c r="D59" s="45"/>
       <c r="E59" s="45"/>
       <c r="F59" s="45"/>
       <c r="G59" s="45"/>
       <c r="H59" s="45"/>
-    </row>
-    <row r="60" spans="2:8" s="35" customFormat="1" ht="42.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I59" s="45"/>
+    </row>
+    <row r="60" spans="2:9" s="35" customFormat="1" ht="42.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B60" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="C60" s="47"/>
+      <c r="C60" s="49"/>
       <c r="D60" s="47"/>
       <c r="E60" s="47"/>
       <c r="F60" s="47"/>
       <c r="G60" s="47"/>
       <c r="H60" s="47"/>
-    </row>
-    <row r="61" spans="2:8" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="I60" s="47"/>
+    </row>
+    <row r="61" spans="2:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B61" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="C61" s="45"/>
+      <c r="C61" s="49"/>
       <c r="D61" s="45"/>
       <c r="E61" s="45"/>
       <c r="F61" s="45"/>
       <c r="G61" s="45"/>
       <c r="H61" s="45"/>
-    </row>
-    <row r="62" spans="2:8" s="50" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I61" s="45"/>
+    </row>
+    <row r="62" spans="2:9" s="50" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B62" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="C62" s="47"/>
+      <c r="C62" s="49"/>
       <c r="D62" s="47"/>
       <c r="E62" s="47"/>
       <c r="F62" s="47"/>
       <c r="G62" s="47"/>
       <c r="H62" s="47"/>
-    </row>
-    <row r="63" spans="2:8" s="35" customFormat="1" ht="44.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I62" s="47"/>
+    </row>
+    <row r="63" spans="2:9" s="35" customFormat="1" ht="44.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B63" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="C63" s="47"/>
+      <c r="C63" s="49"/>
       <c r="D63" s="47"/>
       <c r="E63" s="47"/>
       <c r="F63" s="47"/>
       <c r="G63" s="47"/>
       <c r="H63" s="47"/>
-    </row>
-    <row r="64" spans="2:8" ht="14.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="65" spans="2:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="I63" s="47"/>
+    </row>
+    <row r="64" spans="2:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="65" spans="2:9" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B65" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C65" s="17"/>
+      <c r="C65" s="20"/>
       <c r="D65" s="17"/>
       <c r="E65" s="17"/>
       <c r="F65" s="17"/>
       <c r="G65" s="17"/>
       <c r="H65" s="17"/>
-    </row>
-    <row r="66" spans="2:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I65" s="17"/>
+    </row>
+    <row r="66" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B66" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="C66" s="48" t="s">
+      <c r="C66" s="52"/>
+      <c r="D66" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="D66" s="53"/>
-      <c r="F66" s="52" t="s">
+      <c r="E66" s="53"/>
+      <c r="G66" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="G66" s="48"/>
-      <c r="H66" s="48" t="s">
+      <c r="H66" s="48"/>
+      <c r="I66" s="48" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="67" spans="2:8" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="2:9" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B67" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="C67" s="46"/>
+      <c r="C67" s="58"/>
       <c r="D67" s="46"/>
-      <c r="F67" s="58" t="s">
+      <c r="E67" s="46"/>
+      <c r="G67" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="G67" s="35"/>
       <c r="H67" s="35"/>
-    </row>
-    <row r="68" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I67" s="35"/>
+    </row>
+    <row r="68" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B68" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="C68" s="46"/>
+      <c r="C68" s="58"/>
       <c r="D68" s="46"/>
-      <c r="F68" s="58" t="s">
+      <c r="E68" s="46"/>
+      <c r="G68" s="58" t="s">
         <v>103</v>
       </c>
-      <c r="G68" s="46"/>
       <c r="H68" s="46"/>
-    </row>
-    <row r="69" spans="2:8" ht="12.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I68" s="46"/>
+    </row>
+    <row r="69" spans="2:9" ht="12.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B69" s="58" t="s">
         <v>93</v>
       </c>
-      <c r="C69" s="59"/>
-      <c r="D69" s="46"/>
-      <c r="F69" s="58" t="s">
+      <c r="C69" s="58"/>
+      <c r="D69" s="59"/>
+      <c r="E69" s="46"/>
+      <c r="G69" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="G69" s="46"/>
       <c r="H69" s="46"/>
-    </row>
-    <row r="70" spans="2:8" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I69" s="46"/>
+    </row>
+    <row r="70" spans="2:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B70" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C70" s="46"/>
+      <c r="C70" s="58"/>
       <c r="D70" s="46"/>
-      <c r="F70" s="58" t="s">
+      <c r="E70" s="46"/>
+      <c r="G70" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="G70" s="46"/>
       <c r="H70" s="46"/>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="I70" s="46"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B71" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="C71" s="46"/>
-      <c r="D71" s="54"/>
-      <c r="F71" s="58" t="s">
+      <c r="C71" s="58"/>
+      <c r="D71" s="46"/>
+      <c r="E71" s="54"/>
+      <c r="G71" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="G71" s="46"/>
       <c r="H71" s="46"/>
-    </row>
-    <row r="72" spans="2:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I71" s="46"/>
+    </row>
+    <row r="72" spans="2:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B72" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="C72" s="35"/>
-      <c r="F72" s="58" t="s">
+      <c r="C72" s="58"/>
+      <c r="D72" s="35"/>
+      <c r="G72" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="G72" s="35"/>
       <c r="H72" s="35"/>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="I72" s="35"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B73" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="C73" s="46"/>
+      <c r="C73" s="58"/>
       <c r="D73" s="46"/>
-      <c r="F73" s="58" t="s">
+      <c r="E73" s="46"/>
+      <c r="G73" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="G73" s="46"/>
       <c r="H73" s="46"/>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="I73" s="46"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B74" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="C74" s="46"/>
+      <c r="C74" s="58"/>
       <c r="D74" s="46"/>
-      <c r="F74" s="58" t="s">
+      <c r="E74" s="46"/>
+      <c r="G74" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="G74" s="46"/>
       <c r="H74" s="46"/>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="I74" s="46"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B75" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="C75" s="46"/>
+      <c r="C75" s="58"/>
       <c r="D75" s="46"/>
-      <c r="F75" s="58" t="s">
+      <c r="E75" s="46"/>
+      <c r="G75" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="G75" s="46"/>
       <c r="H75" s="46"/>
-    </row>
-    <row r="77" spans="2:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="78" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I75" s="46"/>
+    </row>
+    <row r="77" spans="2:9" ht="30.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="78" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B78" s="63" t="s">
         <v>109</v>
       </c>
       <c r="C78" s="63"/>
-      <c r="D78" s="38"/>
-      <c r="F78" s="63" t="s">
+      <c r="D78" s="63"/>
+      <c r="E78" s="38"/>
+      <c r="G78" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="G78" s="63"/>
       <c r="H78" s="63"/>
-    </row>
-    <row r="79" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B79" s="55"/>
-      <c r="C79" s="56"/>
-      <c r="F79" s="57"/>
+      <c r="I78" s="63"/>
+    </row>
+    <row r="79" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B79" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="C79" s="55"/>
+      <c r="D79" s="56"/>
       <c r="G79" s="57"/>
       <c r="H79" s="57"/>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="I79" s="57"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B80" s="62" t="s">
         <v>74</v>
       </c>
       <c r="C80" s="62"/>
-      <c r="D80" s="38"/>
-      <c r="F80" s="62" t="s">
+      <c r="D80" s="62"/>
+      <c r="E80" s="38"/>
+      <c r="G80" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="G80" s="62"/>
       <c r="H80" s="62"/>
-    </row>
-    <row r="81" spans="8:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="H81" s="15" t="s">
+      <c r="I80" s="62"/>
+    </row>
+    <row r="81" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I81" s="15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="82" spans="8:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="83" spans="8:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="84" spans="8:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="85" spans="8:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="86" spans="8:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="87" spans="8:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="88" spans="8:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="89" spans="8:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="90" spans="8:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="91" spans="8:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="92" spans="8:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="93" spans="8:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="94" spans="8:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="95" spans="8:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="96" spans="8:8" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="82" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="83" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="84" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="85" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="86" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="87" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="88" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="89" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="90" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="91" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="92" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="93" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="94" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="95" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="96" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="97" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="98" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="99" ht="66" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:I7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="7.874015748031496E-2" right="7.874015748031496E-2" top="0.19685039370078741" bottom="0.19685039370078741" header="0.11811023622047245" footer="0"/>
-  <pageSetup paperSize="9" scale="79" fitToHeight="2" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="77" fitToHeight="2" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="44" max="8" man="1"/>
   </rowBreaks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2520,11 +2691,11 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="99.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B4" s="73" t="s">
@@ -2534,40 +2705,40 @@
       <c r="D4" s="73"/>
     </row>
     <row r="5" spans="2:4" ht="26.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
     </row>
     <row r="6" spans="2:4" s="7" customFormat="1" ht="35.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
     </row>
     <row r="7" spans="2:4" s="8" customFormat="1" ht="35.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
     </row>
     <row r="9" spans="2:4" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="2:4" ht="14.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B11" s="3" t="s">
@@ -2575,25 +2746,25 @@
       </c>
     </row>
     <row r="12" spans="2:4" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
     </row>
     <row r="13" spans="2:4" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="70" t="s">
+      <c r="B13" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="70"/>
-      <c r="D13" s="70"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
     </row>
     <row r="14" spans="2:4" s="7" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="70" t="s">
+      <c r="B14" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
     </row>
     <row r="16" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="73" t="s">
@@ -2603,39 +2774,39 @@
       <c r="D16" s="73"/>
     </row>
     <row r="17" spans="2:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="72" t="s">
+      <c r="B17" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="72"/>
-      <c r="D17" s="72"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
     </row>
     <row r="18" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="70" t="s">
+      <c r="B18" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B19" s="70" t="s">
+      <c r="B19" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B20" s="75" t="s">
+      <c r="B20" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="75"/>
-      <c r="D20" s="75"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="72"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="75"/>
-      <c r="D21" s="75"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B23" s="73" t="s">
@@ -2645,67 +2816,67 @@
       <c r="D23" s="73"/>
     </row>
     <row r="24" spans="2:4" ht="39.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="70" t="s">
+      <c r="B24" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="70"/>
-      <c r="D24" s="70"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
     </row>
     <row r="25" spans="2:4" s="8" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="70" t="s">
+      <c r="B25" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="70"/>
-      <c r="D25" s="70"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
     </row>
     <row r="26" spans="2:4" s="8" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="70" t="s">
+      <c r="B26" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="71"/>
     </row>
     <row r="27" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="70" t="s">
+      <c r="B27" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="70"/>
-      <c r="D27" s="70"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B28" s="75" t="s">
+      <c r="B28" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="75"/>
-      <c r="D28" s="75"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B29" s="75" t="s">
+      <c r="B29" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="75"/>
-      <c r="D29" s="75"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="72"/>
     </row>
     <row r="30" spans="2:4" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="70" t="s">
+      <c r="B30" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
     </row>
     <row r="31" spans="2:4" s="8" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="70" t="s">
+      <c r="B31" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="70"/>
-      <c r="D31" s="70"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="71"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B32" s="75" t="s">
+      <c r="B32" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="72"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B34" s="73" t="s">
@@ -2715,39 +2886,39 @@
       <c r="D34" s="73"/>
     </row>
     <row r="35" spans="2:4" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="70" t="s">
+      <c r="B35" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
     </row>
     <row r="36" spans="2:4" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="70" t="s">
+      <c r="B36" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="70"/>
-      <c r="D36" s="70"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="71"/>
     </row>
     <row r="37" spans="2:4" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="70" t="s">
+      <c r="B37" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="71"/>
     </row>
     <row r="38" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="74" t="s">
+      <c r="B38" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="74"/>
-      <c r="D38" s="74"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="76"/>
     </row>
     <row r="39" spans="2:4" ht="113.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="72" t="s">
+      <c r="B39" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="72"/>
-      <c r="D39" s="72"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="70"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B41" s="73" t="s">
@@ -2757,46 +2928,46 @@
       <c r="D41" s="73"/>
     </row>
     <row r="42" spans="2:4" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="70" t="s">
+      <c r="B42" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="70"/>
-      <c r="D42" s="70"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
     </row>
     <row r="43" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="70" t="s">
+      <c r="B43" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="70"/>
-      <c r="D43" s="70"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="71"/>
     </row>
     <row r="44" spans="2:4" ht="30.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="72" t="s">
+      <c r="B44" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="72"/>
-      <c r="D44" s="72"/>
+      <c r="C44" s="70"/>
+      <c r="D44" s="70"/>
     </row>
     <row r="45" spans="2:4" ht="42.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="72" t="s">
+      <c r="B45" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="72"/>
-      <c r="D45" s="72"/>
+      <c r="C45" s="70"/>
+      <c r="D45" s="70"/>
     </row>
     <row r="46" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="72" t="s">
+      <c r="B46" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="72"/>
-      <c r="D46" s="72"/>
+      <c r="C46" s="70"/>
+      <c r="D46" s="70"/>
     </row>
     <row r="47" spans="2:4" ht="39" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="72" t="s">
+      <c r="B47" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="72"/>
-      <c r="D47" s="72"/>
+      <c r="C47" s="70"/>
+      <c r="D47" s="70"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B49" s="73" t="s">
@@ -2806,60 +2977,60 @@
       <c r="D49" s="73"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B50" s="72" t="s">
+      <c r="B50" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="72"/>
-      <c r="D50" s="72"/>
+      <c r="C50" s="70"/>
+      <c r="D50" s="70"/>
     </row>
     <row r="51" spans="2:4" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="72" t="s">
+      <c r="B51" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="72"/>
-      <c r="D51" s="72"/>
+      <c r="C51" s="70"/>
+      <c r="D51" s="70"/>
     </row>
     <row r="52" spans="2:4" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="70" t="s">
+      <c r="B52" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="70"/>
-      <c r="D52" s="70"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="71"/>
     </row>
     <row r="53" spans="2:4" s="8" customFormat="1" ht="36.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="70" t="s">
+      <c r="B53" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="70"/>
-      <c r="D53" s="70"/>
+      <c r="C53" s="71"/>
+      <c r="D53" s="71"/>
     </row>
     <row r="54" spans="2:4" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B54" s="72" t="s">
+      <c r="B54" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="72"/>
-      <c r="D54" s="72"/>
+      <c r="C54" s="70"/>
+      <c r="D54" s="70"/>
     </row>
     <row r="55" spans="2:4" s="5" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="70" t="s">
+      <c r="B55" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="70"/>
-      <c r="D55" s="70"/>
+      <c r="C55" s="71"/>
+      <c r="D55" s="71"/>
     </row>
     <row r="56" spans="2:4" s="8" customFormat="1" ht="51.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="70" t="s">
+      <c r="B56" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="70"/>
-      <c r="D56" s="70"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="71"/>
     </row>
     <row r="58" spans="2:4" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="71" t="s">
+      <c r="B58" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="71"/>
-      <c r="D58" s="71"/>
+      <c r="C58" s="77"/>
+      <c r="D58" s="77"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B59" s="10" t="s">
@@ -2961,11 +3132,38 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B3:D3"/>
@@ -2978,38 +3176,11 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B64" r:id="rId1" display="mailto:main@sea-wolf.ru" xr:uid="{65C32F44-9D5B-4BC8-B696-A4811EE9907B}"/>

</xml_diff>

<commit_message>
inner contract pictures feature added
</commit_message>
<xml_diff>
--- a/templates/Inner_Contract.xlsx
+++ b/templates/Inner_Contract.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D98FEB6-5F7A-40D0-880E-E6B64F067961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823D40B0-0023-434C-A76E-3DE8F9481181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{1078D20C-27F2-4BD9-B9EF-0CD976B5C671}"/>
   </bookViews>
@@ -20,6 +20,8 @@
     <definedName name="Pg_end">Contract!$I$81</definedName>
     <definedName name="Pg_start">Contract!$B$1</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Contract!$A$2:$J$99</definedName>
+    <definedName name="Seal_seller_start">Contract!$C$78</definedName>
+    <definedName name="Sign_seller_start">Contract!$C$79</definedName>
     <definedName name="Договор_адреса_заголовок">Contract!$B$65</definedName>
     <definedName name="Договор_адреса_покупатель">Contract!$G$66</definedName>
     <definedName name="Договор_адреса_покупатель_адрес">Contract!$G$67</definedName>
@@ -93,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="110">
   <si>
     <t>ДОГОВОР ПОСТАВКИ № 551</t>
   </si>
@@ -1024,7 +1026,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1080,9 +1082,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1181,9 +1180,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1224,28 +1220,31 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1263,99 +1262,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>401834</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>324246</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>32741</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>62705</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="A close-up of a signature&#10;&#10;Description automatically generated">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9D29EF8-0F85-47D4-9E1C-18DDDED87D15}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="515936" y="19478426"/>
-          <a:ext cx="1595438" cy="561975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>745330</xdr:colOff>
-      <xdr:row>77</xdr:row>
-      <xdr:rowOff>104180</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>376237</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>828476</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="A blue circle with two dolphins in it&#10;&#10;Description automatically generated">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ED108FC-6E65-40A9-BFAF-5FF7FCEA6291}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="859432" y="19258360"/>
-          <a:ext cx="1595438" cy="1547812"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1680,15 +1586,15 @@
   </sheetPr>
   <dimension ref="B1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A73" zoomScale="96" zoomScaleNormal="100" zoomScaleSheetLayoutView="96" workbookViewId="0">
-      <selection activeCell="H99" sqref="H99"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A62" zoomScale="96" zoomScaleNormal="100" zoomScaleSheetLayoutView="96" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="1.59765625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="27.53125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="12.19921875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" style="15" customWidth="1"/>
     <col min="4" max="4" width="15" style="15" customWidth="1"/>
     <col min="5" max="5" width="10.265625" style="15" customWidth="1"/>
     <col min="6" max="6" width="6.59765625" style="15" customWidth="1"/>
@@ -1705,16 +1611,16 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="23.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="2:9" s="18" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="17" t="s">
@@ -1724,22 +1630,22 @@
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
-      <c r="H3" s="66" t="s">
+      <c r="H3" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="66"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="2:9" ht="71.349999999999994" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
     </row>
     <row r="5" spans="2:9" ht="5.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="19"/>
@@ -1752,510 +1658,510 @@
       <c r="I5" s="19"/>
     </row>
     <row r="6" spans="2:9" s="18" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
     </row>
     <row r="7" spans="2:9" ht="29.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-    </row>
-    <row r="8" spans="2:9" s="24" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="21" t="s">
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
+    </row>
+    <row r="8" spans="2:9" s="23" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="61" t="s">
+      <c r="C8" s="59"/>
+      <c r="D8" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="61"/>
-      <c r="F8" s="22" t="s">
+      <c r="E8" s="59"/>
+      <c r="F8" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="H8" s="61" t="s">
+      <c r="H8" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="I8" s="64"/>
-    </row>
-    <row r="9" spans="2:9" s="24" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="25" t="s">
+      <c r="I8" s="62"/>
+    </row>
+    <row r="9" spans="2:9" s="23" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="28" t="s">
+      <c r="C9" s="25"/>
+      <c r="D9" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="26" t="s">
+      <c r="E9" s="27"/>
+      <c r="F9" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="H9" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="29"/>
-    </row>
-    <row r="10" spans="2:9" s="35" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="30" t="s">
+      <c r="I9" s="28"/>
+    </row>
+    <row r="10" spans="2:9" s="34" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="33" t="s">
+      <c r="C10" s="30"/>
+      <c r="D10" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="31" t="s">
+      <c r="E10" s="32"/>
+      <c r="F10" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="33" t="s">
+      <c r="H10" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="I10" s="34"/>
+      <c r="I10" s="33"/>
     </row>
     <row r="11" spans="2:9" ht="20.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
     </row>
     <row r="12" spans="2:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
     </row>
     <row r="13" spans="2:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="16"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
     </row>
     <row r="14" spans="2:9" ht="22.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="18"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="40"/>
-    </row>
-    <row r="15" spans="2:9" s="35" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="21" t="s">
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
+    </row>
+    <row r="15" spans="2:9" s="34" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22" t="s">
+      <c r="C15" s="59"/>
+      <c r="D15" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22" t="s">
+      <c r="E15" s="59"/>
+      <c r="F15" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="22" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="2:9" s="35" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="25" t="s">
+    <row r="16" spans="2:9" s="34" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="28" t="s">
+      <c r="C16" s="25"/>
+      <c r="D16" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="28"/>
-      <c r="F16" s="26" t="s">
+      <c r="E16" s="27"/>
+      <c r="F16" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="I16" s="41">
+      <c r="I16" s="40">
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="2:9" s="35" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="30" t="s">
+    <row r="17" spans="2:9" s="34" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="33" t="s">
+      <c r="C17" s="30"/>
+      <c r="D17" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="33"/>
-      <c r="F17" s="31" t="s">
+      <c r="E17" s="32"/>
+      <c r="F17" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="G17" s="32" t="s">
+      <c r="G17" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="31" t="s">
+      <c r="H17" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="I17" s="42">
+      <c r="I17" s="41">
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="2:9" s="24" customFormat="1" ht="36.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="36" t="s">
+    <row r="18" spans="2:9" s="23" customFormat="1" ht="36.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-    </row>
-    <row r="19" spans="2:9" s="24" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-    </row>
-    <row r="20" spans="2:9" s="24" customFormat="1" ht="15.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="43" t="s">
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+    </row>
+    <row r="19" spans="2:9" s="23" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+    </row>
+    <row r="20" spans="2:9" s="23" customFormat="1" ht="15.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="43"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
     </row>
     <row r="21" spans="2:9" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="37"/>
+      <c r="C21" s="36"/>
     </row>
     <row r="22" spans="2:9" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
     </row>
     <row r="23" spans="2:9" ht="16.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
     </row>
     <row r="24" spans="2:9" ht="16.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
     </row>
     <row r="25" spans="2:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B26" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="16"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
       <c r="I26" s="16"/>
     </row>
     <row r="27" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="49" t="s">
+      <c r="B27" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="49"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
     </row>
     <row r="28" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="49"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
     </row>
     <row r="29" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="49" t="s">
+      <c r="B29" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C29" s="49"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
     </row>
     <row r="30" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="49" t="s">
+      <c r="B30" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="49"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
     </row>
     <row r="31" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="49" t="s">
+      <c r="B31" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="49"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-    </row>
-    <row r="32" spans="2:9" s="35" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="49" t="s">
+      <c r="C31" s="48"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+    </row>
+    <row r="32" spans="2:9" s="34" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C32" s="49"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-    </row>
-    <row r="33" spans="2:9" s="35" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="49" t="s">
+      <c r="C32" s="48"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+    </row>
+    <row r="33" spans="2:9" s="34" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="49"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
     </row>
     <row r="34" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C34" s="49"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
     </row>
     <row r="35" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C35" s="49"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
     </row>
     <row r="36" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="49" t="s">
+      <c r="B36" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="49"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-    </row>
-    <row r="37" spans="2:9" s="35" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="49" t="s">
+      <c r="C36" s="48"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+    </row>
+    <row r="37" spans="2:9" s="34" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C37" s="49"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="47"/>
-      <c r="I37" s="47"/>
-    </row>
-    <row r="38" spans="2:9" s="35" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="49" t="s">
+      <c r="C37" s="48"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+    </row>
+    <row r="38" spans="2:9" s="34" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C38" s="49"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
-      <c r="I38" s="47"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
     </row>
     <row r="39" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="49" t="s">
+      <c r="B39" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="49"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="47"/>
-      <c r="I39" s="47"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B41" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C41" s="16"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="48"/>
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="47"/>
     </row>
     <row r="42" spans="2:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="49" t="s">
+      <c r="B42" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="C42" s="49"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="47"/>
-      <c r="I42" s="47"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
     </row>
     <row r="43" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="49" t="s">
+      <c r="B43" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="49"/>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="47"/>
-      <c r="I43" s="47"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="46"/>
     </row>
     <row r="44" spans="2:9" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="49" t="s">
+      <c r="B44" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="C44" s="49"/>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
-      <c r="H44" s="47"/>
-      <c r="I44" s="47"/>
+      <c r="C44" s="48"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="46"/>
     </row>
     <row r="45" spans="2:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="49" t="s">
+      <c r="B45" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="C45" s="49"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="47"/>
-      <c r="F45" s="47"/>
-      <c r="G45" s="47"/>
-      <c r="H45" s="47"/>
-      <c r="I45" s="47"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="46"/>
+      <c r="I45" s="46"/>
     </row>
     <row r="46" spans="2:9" ht="86.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="49" t="s">
+      <c r="B46" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="C46" s="49"/>
-      <c r="D46" s="47"/>
-      <c r="E46" s="47"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="47"/>
-      <c r="H46" s="47"/>
-      <c r="I46" s="47"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="46"/>
     </row>
     <row r="47" spans="2:9" ht="12.85" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="48" spans="2:9" x14ac:dyDescent="0.4">
@@ -2263,84 +2169,84 @@
         <v>32</v>
       </c>
       <c r="C48" s="16"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="48"/>
-      <c r="I48" s="48"/>
-    </row>
-    <row r="49" spans="2:9" s="50" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B49" s="49" t="s">
+      <c r="D48" s="47"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="47"/>
+      <c r="I48" s="47"/>
+    </row>
+    <row r="49" spans="2:9" s="49" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B49" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="49"/>
-      <c r="D49" s="47"/>
-      <c r="E49" s="47"/>
-      <c r="F49" s="47"/>
-      <c r="G49" s="47"/>
-      <c r="H49" s="47"/>
-      <c r="I49" s="47"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="46"/>
+      <c r="G49" s="46"/>
+      <c r="H49" s="46"/>
+      <c r="I49" s="46"/>
     </row>
     <row r="50" spans="2:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="49" t="s">
+      <c r="B50" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="49"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="45"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="45"/>
+      <c r="C50" s="48"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="44"/>
+      <c r="H50" s="44"/>
+      <c r="I50" s="44"/>
     </row>
     <row r="51" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="49" t="s">
+      <c r="B51" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="C51" s="49"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="47"/>
+      <c r="C51" s="48"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="46"/>
     </row>
     <row r="52" spans="2:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="49" t="s">
+      <c r="B52" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C52" s="49"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="47"/>
-      <c r="I52" s="47"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="46"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="46"/>
+      <c r="G52" s="46"/>
+      <c r="H52" s="46"/>
+      <c r="I52" s="46"/>
     </row>
     <row r="53" spans="2:9" ht="41.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="49" t="s">
+      <c r="B53" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="C53" s="49"/>
-      <c r="D53" s="47"/>
-      <c r="E53" s="47"/>
-      <c r="F53" s="47"/>
-      <c r="G53" s="47"/>
-      <c r="H53" s="47"/>
-      <c r="I53" s="47"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="46"/>
+      <c r="F53" s="46"/>
+      <c r="G53" s="46"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="46"/>
     </row>
     <row r="54" spans="2:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B54" s="49" t="s">
+      <c r="B54" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C54" s="49"/>
-      <c r="D54" s="47"/>
-      <c r="E54" s="47"/>
-      <c r="F54" s="47"/>
-      <c r="G54" s="47"/>
-      <c r="H54" s="47"/>
-      <c r="I54" s="47"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="46"/>
     </row>
     <row r="55" spans="2:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="56" spans="2:9" x14ac:dyDescent="0.4">
@@ -2348,90 +2254,90 @@
         <v>43</v>
       </c>
       <c r="C56" s="16"/>
-      <c r="D56" s="48"/>
-      <c r="E56" s="48"/>
-      <c r="F56" s="48"/>
-      <c r="G56" s="48"/>
-      <c r="H56" s="48"/>
-      <c r="I56" s="48"/>
+      <c r="D56" s="47"/>
+      <c r="E56" s="47"/>
+      <c r="F56" s="47"/>
+      <c r="G56" s="47"/>
+      <c r="H56" s="47"/>
+      <c r="I56" s="47"/>
     </row>
     <row r="57" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B57" s="49" t="s">
+      <c r="B57" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C57" s="49"/>
-      <c r="D57" s="47"/>
-      <c r="E57" s="47"/>
-      <c r="F57" s="47"/>
-      <c r="G57" s="47"/>
-      <c r="H57" s="47"/>
-      <c r="I57" s="47"/>
-    </row>
-    <row r="58" spans="2:9" s="45" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="49" t="s">
+      <c r="C57" s="48"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="46"/>
+      <c r="I57" s="46"/>
+    </row>
+    <row r="58" spans="2:9" s="44" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B58" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="C58" s="49"/>
+      <c r="C58" s="48"/>
     </row>
     <row r="59" spans="2:9" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B59" s="49" t="s">
+      <c r="B59" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C59" s="49"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="45"/>
-      <c r="F59" s="45"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="45"/>
-      <c r="I59" s="45"/>
-    </row>
-    <row r="60" spans="2:9" s="35" customFormat="1" ht="42.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B60" s="49" t="s">
+      <c r="C59" s="48"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="44"/>
+      <c r="H59" s="44"/>
+      <c r="I59" s="44"/>
+    </row>
+    <row r="60" spans="2:9" s="34" customFormat="1" ht="42.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B60" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="C60" s="49"/>
-      <c r="D60" s="47"/>
-      <c r="E60" s="47"/>
-      <c r="F60" s="47"/>
-      <c r="G60" s="47"/>
-      <c r="H60" s="47"/>
-      <c r="I60" s="47"/>
-    </row>
-    <row r="61" spans="2:9" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B61" s="49" t="s">
+      <c r="C60" s="48"/>
+      <c r="D60" s="46"/>
+      <c r="E60" s="46"/>
+      <c r="F60" s="46"/>
+      <c r="G60" s="46"/>
+      <c r="H60" s="46"/>
+      <c r="I60" s="46"/>
+    </row>
+    <row r="61" spans="2:9" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B61" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="C61" s="49"/>
-      <c r="D61" s="45"/>
-      <c r="E61" s="45"/>
-      <c r="F61" s="45"/>
-      <c r="G61" s="45"/>
-      <c r="H61" s="45"/>
-      <c r="I61" s="45"/>
-    </row>
-    <row r="62" spans="2:9" s="50" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="49" t="s">
+      <c r="C61" s="48"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="44"/>
+      <c r="H61" s="44"/>
+      <c r="I61" s="44"/>
+    </row>
+    <row r="62" spans="2:9" s="49" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B62" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="C62" s="49"/>
-      <c r="D62" s="47"/>
-      <c r="E62" s="47"/>
-      <c r="F62" s="47"/>
-      <c r="G62" s="47"/>
-      <c r="H62" s="47"/>
-      <c r="I62" s="47"/>
-    </row>
-    <row r="63" spans="2:9" s="35" customFormat="1" ht="44.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B63" s="49" t="s">
+      <c r="C62" s="48"/>
+      <c r="D62" s="46"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="46"/>
+      <c r="G62" s="46"/>
+      <c r="H62" s="46"/>
+      <c r="I62" s="46"/>
+    </row>
+    <row r="63" spans="2:9" s="34" customFormat="1" ht="44.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B63" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="C63" s="49"/>
-      <c r="D63" s="47"/>
-      <c r="E63" s="47"/>
-      <c r="F63" s="47"/>
-      <c r="G63" s="47"/>
-      <c r="H63" s="47"/>
-      <c r="I63" s="47"/>
+      <c r="C63" s="48"/>
+      <c r="D63" s="46"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="46"/>
+      <c r="G63" s="46"/>
+      <c r="H63" s="46"/>
+      <c r="I63" s="46"/>
     </row>
     <row r="64" spans="2:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="65" spans="2:9" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -2447,198 +2353,199 @@
       <c r="I65" s="17"/>
     </row>
     <row r="66" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B66" s="52" t="s">
+      <c r="B66" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="C66" s="52"/>
-      <c r="D66" s="48" t="s">
+      <c r="C66" s="51"/>
+      <c r="D66" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="E66" s="53"/>
-      <c r="G66" s="52" t="s">
+      <c r="E66" s="52"/>
+      <c r="G66" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="H66" s="48"/>
-      <c r="I66" s="48" t="s">
+      <c r="H66" s="47"/>
+      <c r="I66" s="47" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="67" spans="2:9" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B67" s="58" t="s">
+      <c r="B67" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="C67" s="58"/>
-      <c r="D67" s="46"/>
-      <c r="E67" s="46"/>
-      <c r="G67" s="58" t="s">
+      <c r="C67" s="56"/>
+      <c r="D67" s="45"/>
+      <c r="E67" s="45"/>
+      <c r="G67" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="H67" s="35"/>
-      <c r="I67" s="35"/>
+      <c r="H67" s="34"/>
+      <c r="I67" s="34"/>
     </row>
     <row r="68" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B68" s="58" t="s">
+      <c r="B68" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="C68" s="58"/>
-      <c r="D68" s="46"/>
-      <c r="E68" s="46"/>
-      <c r="G68" s="58" t="s">
+      <c r="C68" s="56"/>
+      <c r="D68" s="45"/>
+      <c r="E68" s="45"/>
+      <c r="G68" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="H68" s="46"/>
-      <c r="I68" s="46"/>
+      <c r="H68" s="45"/>
+      <c r="I68" s="45"/>
     </row>
     <row r="69" spans="2:9" ht="12.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B69" s="58" t="s">
+      <c r="B69" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="C69" s="58"/>
-      <c r="D69" s="59"/>
-      <c r="E69" s="46"/>
-      <c r="G69" s="58" t="s">
+      <c r="C69" s="56"/>
+      <c r="D69" s="57"/>
+      <c r="E69" s="45"/>
+      <c r="G69" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="H69" s="46"/>
-      <c r="I69" s="46"/>
+      <c r="H69" s="45"/>
+      <c r="I69" s="45"/>
     </row>
     <row r="70" spans="2:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B70" s="58" t="s">
+      <c r="B70" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="C70" s="58"/>
-      <c r="D70" s="46"/>
-      <c r="E70" s="46"/>
-      <c r="G70" s="58" t="s">
+      <c r="C70" s="56"/>
+      <c r="D70" s="45"/>
+      <c r="E70" s="45"/>
+      <c r="G70" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="H70" s="46"/>
-      <c r="I70" s="46"/>
-    </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B71" s="58" t="s">
+      <c r="H70" s="45"/>
+      <c r="I70" s="45"/>
+    </row>
+    <row r="71" spans="2:9" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="B71" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="C71" s="58"/>
-      <c r="D71" s="46"/>
-      <c r="E71" s="54"/>
-      <c r="G71" s="58" t="s">
+      <c r="C71" s="56"/>
+      <c r="D71" s="45"/>
+      <c r="E71" s="53"/>
+      <c r="G71" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="H71" s="46"/>
-      <c r="I71" s="46"/>
+      <c r="H71" s="45"/>
+      <c r="I71" s="45"/>
     </row>
     <row r="72" spans="2:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B72" s="58" t="s">
+      <c r="B72" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="C72" s="58"/>
-      <c r="D72" s="35"/>
-      <c r="G72" s="58" t="s">
+      <c r="C72" s="56"/>
+      <c r="D72" s="34"/>
+      <c r="G72" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="H72" s="35"/>
-      <c r="I72" s="35"/>
+      <c r="H72" s="34"/>
+      <c r="I72" s="34"/>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B73" s="58" t="s">
+      <c r="B73" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="C73" s="58"/>
-      <c r="D73" s="46"/>
-      <c r="E73" s="46"/>
-      <c r="G73" s="58" t="s">
+      <c r="C73" s="56"/>
+      <c r="D73" s="45"/>
+      <c r="E73" s="45"/>
+      <c r="G73" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="H73" s="46"/>
-      <c r="I73" s="46"/>
+      <c r="H73" s="45"/>
+      <c r="I73" s="45"/>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B74" s="58" t="s">
+      <c r="B74" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="C74" s="58"/>
-      <c r="D74" s="46"/>
-      <c r="E74" s="46"/>
-      <c r="G74" s="58" t="s">
+      <c r="C74" s="56"/>
+      <c r="D74" s="45"/>
+      <c r="E74" s="45"/>
+      <c r="G74" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="H74" s="46"/>
-      <c r="I74" s="46"/>
+      <c r="H74" s="45"/>
+      <c r="I74" s="45"/>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B75" s="58" t="s">
+      <c r="B75" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="C75" s="58"/>
-      <c r="D75" s="46"/>
-      <c r="E75" s="46"/>
-      <c r="G75" s="58" t="s">
+      <c r="C75" s="56"/>
+      <c r="D75" s="45"/>
+      <c r="E75" s="45"/>
+      <c r="G75" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="H75" s="46"/>
-      <c r="I75" s="46"/>
+      <c r="H75" s="45"/>
+      <c r="I75" s="45"/>
     </row>
     <row r="77" spans="2:9" ht="30.85" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="78" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B78" s="63" t="s">
+      <c r="B78" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="C78" s="63"/>
-      <c r="D78" s="63"/>
-      <c r="E78" s="38"/>
-      <c r="G78" s="63" t="s">
+      <c r="C78" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D78" s="61"/>
+      <c r="E78" s="37"/>
+      <c r="G78" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="H78" s="63"/>
-      <c r="I78" s="63"/>
-    </row>
-    <row r="79" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B79" s="55" t="s">
+      <c r="H78" s="61"/>
+      <c r="I78" s="61"/>
+    </row>
+    <row r="79" spans="2:9" ht="20.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C79" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C79" s="55"/>
-      <c r="D79" s="56"/>
-      <c r="G79" s="57"/>
-      <c r="H79" s="57"/>
-      <c r="I79" s="57"/>
+      <c r="D79" s="54"/>
+      <c r="G79" s="55"/>
+      <c r="H79" s="55"/>
+      <c r="I79" s="55"/>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B80" s="62" t="s">
+      <c r="B80" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="C80" s="62"/>
-      <c r="D80" s="62"/>
-      <c r="E80" s="38"/>
-      <c r="G80" s="62" t="s">
+      <c r="C80" s="60"/>
+      <c r="D80" s="60"/>
+      <c r="E80" s="37"/>
+      <c r="G80" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="H80" s="62"/>
-      <c r="I80" s="62"/>
-    </row>
-    <row r="81" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="H80" s="60"/>
+      <c r="I80" s="60"/>
+    </row>
+    <row r="81" spans="9:9" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="I81" s="15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="82" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="83" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="84" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="85" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="86" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="87" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="88" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="89" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="90" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="91" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="92" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="93" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="94" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="95" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="96" spans="9:9" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="97" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="98" ht="0.4" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="99" ht="66" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="82" spans="9:9" ht="35.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="83" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="84" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="85" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="86" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="87" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="88" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="89" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="90" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="91" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="92" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="93" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="94" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="95" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="96" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="97" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="98" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="99" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B4:I4"/>
@@ -2653,7 +2560,6 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="44" max="8" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2676,11 +2582,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="23.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
     </row>
     <row r="2" spans="2:4" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
@@ -2698,39 +2604,39 @@
       <c r="D3" s="74"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
     </row>
     <row r="5" spans="2:4" ht="26.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
     </row>
     <row r="6" spans="2:4" s="7" customFormat="1" ht="35.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
     </row>
     <row r="7" spans="2:4" s="8" customFormat="1" ht="35.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
     </row>
     <row r="9" spans="2:4" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="2:4" ht="14.65" customHeight="1" x14ac:dyDescent="0.4">
@@ -2746,32 +2652,32 @@
       </c>
     </row>
     <row r="12" spans="2:4" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="68" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
     </row>
     <row r="13" spans="2:4" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
     </row>
     <row r="14" spans="2:4" s="7" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
     </row>
     <row r="16" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="73" t="s">
+      <c r="B16" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="71"/>
     </row>
     <row r="17" spans="2:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="70" t="s">
@@ -2781,137 +2687,137 @@
       <c r="D17" s="70"/>
     </row>
     <row r="18" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="71" t="s">
+      <c r="B18" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B19" s="71" t="s">
+      <c r="B19" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="68"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B20" s="72" t="s">
+      <c r="B20" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="72"/>
-      <c r="D20" s="72"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B21" s="72" t="s">
+      <c r="B21" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
     </row>
     <row r="24" spans="2:4" ht="39.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="71" t="s">
+      <c r="B24" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
     </row>
     <row r="25" spans="2:4" s="8" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="71" t="s">
+      <c r="B25" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="71"/>
-      <c r="D25" s="71"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
     </row>
     <row r="26" spans="2:4" s="8" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="71" t="s">
+      <c r="B26" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="71"/>
-      <c r="D26" s="71"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
     </row>
     <row r="27" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="71" t="s">
+      <c r="B27" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="71"/>
-      <c r="D27" s="71"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B28" s="72" t="s">
+      <c r="B28" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B29" s="72" t="s">
+      <c r="B29" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="72"/>
-      <c r="D29" s="72"/>
+      <c r="C29" s="73"/>
+      <c r="D29" s="73"/>
     </row>
     <row r="30" spans="2:4" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="71" t="s">
+      <c r="B30" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="71"/>
-      <c r="D30" s="71"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="68"/>
     </row>
     <row r="31" spans="2:4" s="8" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="71" t="s">
+      <c r="B31" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="71"/>
-      <c r="D31" s="71"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="68"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B32" s="72" t="s">
+      <c r="B32" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
+      <c r="C32" s="73"/>
+      <c r="D32" s="73"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B34" s="73" t="s">
+      <c r="B34" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
     </row>
     <row r="35" spans="2:4" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="71" t="s">
+      <c r="B35" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="71"/>
-      <c r="D35" s="71"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="68"/>
     </row>
     <row r="36" spans="2:4" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="71" t="s">
+      <c r="B36" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="71"/>
-      <c r="D36" s="71"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="68"/>
     </row>
     <row r="37" spans="2:4" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="71" t="s">
+      <c r="B37" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="71"/>
-      <c r="D37" s="71"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="68"/>
     </row>
     <row r="38" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="76" t="s">
+      <c r="B38" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="76"/>
-      <c r="D38" s="76"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
     </row>
     <row r="39" spans="2:4" ht="113.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B39" s="70" t="s">
@@ -2921,25 +2827,25 @@
       <c r="D39" s="70"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B41" s="73" t="s">
+      <c r="B41" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="73"/>
-      <c r="D41" s="73"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
     </row>
     <row r="42" spans="2:4" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="71" t="s">
+      <c r="B42" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="71"/>
-      <c r="D42" s="71"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="68"/>
     </row>
     <row r="43" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="71" t="s">
+      <c r="B43" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="71"/>
-      <c r="D43" s="71"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="68"/>
     </row>
     <row r="44" spans="2:4" ht="30.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B44" s="70" t="s">
@@ -2970,11 +2876,11 @@
       <c r="D47" s="70"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B49" s="73" t="s">
+      <c r="B49" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="73"/>
-      <c r="D49" s="73"/>
+      <c r="C49" s="71"/>
+      <c r="D49" s="71"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B50" s="70" t="s">
@@ -2991,18 +2897,18 @@
       <c r="D51" s="70"/>
     </row>
     <row r="52" spans="2:4" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="71" t="s">
+      <c r="B52" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="71"/>
-      <c r="D52" s="71"/>
+      <c r="C52" s="68"/>
+      <c r="D52" s="68"/>
     </row>
     <row r="53" spans="2:4" s="8" customFormat="1" ht="36.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="71" t="s">
+      <c r="B53" s="68" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="71"/>
-      <c r="D53" s="71"/>
+      <c r="C53" s="68"/>
+      <c r="D53" s="68"/>
     </row>
     <row r="54" spans="2:4" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B54" s="70" t="s">
@@ -3012,25 +2918,25 @@
       <c r="D54" s="70"/>
     </row>
     <row r="55" spans="2:4" s="5" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="71" t="s">
+      <c r="B55" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="71"/>
-      <c r="D55" s="71"/>
+      <c r="C55" s="68"/>
+      <c r="D55" s="68"/>
     </row>
     <row r="56" spans="2:4" s="8" customFormat="1" ht="51.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="71" t="s">
+      <c r="B56" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="71"/>
-      <c r="D56" s="71"/>
+      <c r="C56" s="68"/>
+      <c r="D56" s="68"/>
     </row>
     <row r="58" spans="2:4" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="77" t="s">
+      <c r="B58" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="77"/>
-      <c r="D58" s="77"/>
+      <c r="C58" s="69"/>
+      <c r="D58" s="69"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B59" s="10" t="s">
@@ -3132,38 +3038,11 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B3:D3"/>
@@ -3176,11 +3055,38 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B64" r:id="rId1" display="mailto:main@sea-wolf.ru" xr:uid="{65C32F44-9D5B-4BC8-B696-A4811EE9907B}"/>

</xml_diff>

<commit_message>
inner contract live product fixed
</commit_message>
<xml_diff>
--- a/templates/Inner_Contract.xlsx
+++ b/templates/Inner_Contract.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823D40B0-0023-434C-A76E-3DE8F9481181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC66E72-C6BA-4DE4-B6EC-907D3B0CAB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{1078D20C-27F2-4BD9-B9EF-0CD976B5C671}"/>
   </bookViews>
@@ -17,62 +17,72 @@
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Pg_end">Contract!$I$81</definedName>
+    <definedName name="Pg_end">Contract!$I$86</definedName>
     <definedName name="Pg_start">Contract!$B$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Contract!$A$2:$J$99</definedName>
-    <definedName name="Seal_seller_start">Contract!$C$78</definedName>
-    <definedName name="Sign_seller_start">Contract!$C$79</definedName>
-    <definedName name="Договор_адреса_заголовок">Contract!$B$65</definedName>
-    <definedName name="Договор_адреса_покупатель">Contract!$G$66</definedName>
-    <definedName name="Договор_адреса_покупатель_адрес">Contract!$G$67</definedName>
-    <definedName name="Договор_адреса_покупатель_банк">Contract!$G$72</definedName>
-    <definedName name="Договор_адреса_покупатель_бик">Contract!$G$73</definedName>
-    <definedName name="Договор_адреса_покупатель_должность">Contract!$G$78</definedName>
-    <definedName name="Договор_адреса_покупатель_инн">Contract!$G$70</definedName>
-    <definedName name="Договор_адреса_покупатель_конец">Contract!$I$66</definedName>
-    <definedName name="Договор_адреса_покупатель_кс">Contract!$G$74</definedName>
-    <definedName name="Договор_адреса_покупатель_огрн">Contract!$G$71</definedName>
-    <definedName name="Договор_адреса_покупатель_почта">Contract!$G$69</definedName>
-    <definedName name="Договор_адреса_покупатель_рс">Contract!$G$75</definedName>
-    <definedName name="Договор_адреса_покупатель_тел">Contract!$G$68</definedName>
-    <definedName name="Договор_адреса_покупатель_фио">Contract!$G$80</definedName>
-    <definedName name="Договор_адреса_поставщик">Contract!$B$66</definedName>
-    <definedName name="Договор_адреса_поставщик_адрес">Contract!$B$67</definedName>
-    <definedName name="Договор_адреса_поставщик_банк">Contract!$B$72</definedName>
-    <definedName name="Договор_адреса_поставщик_бик">Contract!$B$73</definedName>
-    <definedName name="Договор_адреса_поставщик_должность">Contract!$B$78</definedName>
-    <definedName name="Договор_адреса_поставщик_инн">Contract!$B$70</definedName>
-    <definedName name="Договор_адреса_поставщик_конец">Contract!$D$66</definedName>
-    <definedName name="Договор_адреса_поставщик_кс">Contract!$B$74</definedName>
-    <definedName name="Договор_адреса_поставщик_огрн">Contract!$B$71</definedName>
-    <definedName name="Договор_адреса_поставщик_почта">Contract!$B$69</definedName>
-    <definedName name="Договор_адреса_поставщик_рс">Contract!$B$75</definedName>
-    <definedName name="Договор_адреса_поставщик_тел">Contract!$B$68</definedName>
-    <definedName name="Договор_адреса_поставщик_фио">Contract!$B$80</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Contract!$A$2:$J$104</definedName>
+    <definedName name="Seal_seller_start">Contract!$C$83</definedName>
+    <definedName name="Sign_seller_start">Contract!$C$84</definedName>
+    <definedName name="Дата_выпуска">Contract!$B$24</definedName>
+    <definedName name="Договор_адреса_заголовок">Contract!$B$70</definedName>
+    <definedName name="Договор_адреса_покупатель">Contract!$G$71</definedName>
+    <definedName name="Договор_адреса_покупатель_адрес">Contract!$G$72</definedName>
+    <definedName name="Договор_адреса_покупатель_банк">Contract!$G$77</definedName>
+    <definedName name="Договор_адреса_покупатель_бик">Contract!$G$78</definedName>
+    <definedName name="Договор_адреса_покупатель_должность">Contract!$G$83</definedName>
+    <definedName name="Договор_адреса_покупатель_инн">Contract!$G$75</definedName>
+    <definedName name="Договор_адреса_покупатель_конец">Contract!$I$71</definedName>
+    <definedName name="Договор_адреса_покупатель_кс">Contract!$G$79</definedName>
+    <definedName name="Договор_адреса_покупатель_огрн">Contract!$G$76</definedName>
+    <definedName name="Договор_адреса_покупатель_почта">Contract!$G$74</definedName>
+    <definedName name="Договор_адреса_покупатель_рс">Contract!$G$80</definedName>
+    <definedName name="Договор_адреса_покупатель_тел">Contract!$G$73</definedName>
+    <definedName name="Договор_адреса_покупатель_фио">Contract!$G$85</definedName>
+    <definedName name="Договор_адреса_поставщик">Contract!$B$71</definedName>
+    <definedName name="Договор_адреса_поставщик_адрес">Contract!$B$72</definedName>
+    <definedName name="Договор_адреса_поставщик_банк">Contract!$B$77</definedName>
+    <definedName name="Договор_адреса_поставщик_бик">Contract!$B$78</definedName>
+    <definedName name="Договор_адреса_поставщик_должность">Contract!$B$83</definedName>
+    <definedName name="Договор_адреса_поставщик_инн">Contract!$B$75</definedName>
+    <definedName name="Договор_адреса_поставщик_конец">Contract!$D$71</definedName>
+    <definedName name="Договор_адреса_поставщик_кс">Contract!$B$79</definedName>
+    <definedName name="Договор_адреса_поставщик_огрн">Contract!$B$76</definedName>
+    <definedName name="Договор_адреса_поставщик_почта">Contract!$B$74</definedName>
+    <definedName name="Договор_адреса_поставщик_рс">Contract!$B$80</definedName>
+    <definedName name="Договор_адреса_поставщик_тел">Contract!$B$73</definedName>
+    <definedName name="Договор_адреса_поставщик_фио">Contract!$B$85</definedName>
     <definedName name="Договор_дата">Contract!$H$3</definedName>
-    <definedName name="Договор_доставка">Contract!$B$33</definedName>
+    <definedName name="Договор_доставка">Contract!$B$38</definedName>
+    <definedName name="Договор_доставка_FCA">Contract!$B$28</definedName>
     <definedName name="Договор_качество_конец">Contract!#REF!</definedName>
     <definedName name="Договор_качество_начало">Contract!#REF!</definedName>
     <definedName name="Договор_конец_предмет">Contract!$B$11</definedName>
-    <definedName name="Договор_Меркурий">Contract!$B$39</definedName>
-    <definedName name="Договор_Меркурий_EXW">Contract!$B$31</definedName>
-    <definedName name="Договор_момент_приемки">Contract!$B$37</definedName>
-    <definedName name="Договор_момент_приемки_EXW">Contract!$B$30</definedName>
+    <definedName name="Договор_Меркурий">Contract!$B$44</definedName>
+    <definedName name="Договор_Меркурий_EXW">Contract!$B$36</definedName>
+    <definedName name="Договор_Меркурий_FCA">Contract!$B$31</definedName>
+    <definedName name="Договор_момент_приемки">Contract!$B$42</definedName>
+    <definedName name="Договор_момент_приемки_EXW">Contract!$B$35</definedName>
+    <definedName name="Договор_момент_приемки_FCA">Contract!$B$30</definedName>
     <definedName name="Договор_номер">Contract!$B$2</definedName>
     <definedName name="Договор_оплата_дата">Contract!$B$27</definedName>
-    <definedName name="Договор_ответственность">Contract!$B$41</definedName>
-    <definedName name="Договор_передача_EXW">Contract!$B$28</definedName>
-    <definedName name="Договор_подход_дата">Contract!$B$32</definedName>
+    <definedName name="Договор_ответственность">Contract!$B$46</definedName>
+    <definedName name="Договор_передача_EXW">Contract!$B$33</definedName>
+    <definedName name="Договор_подход_дата">Contract!$B$37</definedName>
+    <definedName name="Договор_право_собственности_FCA">Contract!$B$32</definedName>
     <definedName name="Договор_предмет_массив">Contract!$B$9</definedName>
-    <definedName name="Договор_приемка_EXW">Contract!$B$29</definedName>
-    <definedName name="Договор_приемка_товара">Contract!$B$34</definedName>
-    <definedName name="Договор_приемка_товара_ВСД">Contract!$B$38</definedName>
-    <definedName name="Договор_приемка_товара_качество">Contract!$B$36</definedName>
-    <definedName name="Договор_приемка_товара_количество">Contract!$B$35</definedName>
+    <definedName name="Договор_приемка_EXW">Contract!$B$34</definedName>
+    <definedName name="Договор_приемка_товара">Contract!$B$39</definedName>
+    <definedName name="Договор_приемка_товара_FCA">Contract!$B$29</definedName>
+    <definedName name="Договор_приемка_товара_ВСД">Contract!$B$43</definedName>
+    <definedName name="Договор_приемка_товара_качество">Contract!$B$41</definedName>
+    <definedName name="Договор_приемка_товара_количество">Contract!$B$40</definedName>
     <definedName name="Договор_стороны">Contract!$B$4</definedName>
     <definedName name="Договор_цена_всего">Contract!$B$18</definedName>
     <definedName name="Договор_цена_массив">Contract!$B$16</definedName>
     <definedName name="Договор_цена_начало">Contract!$B$14</definedName>
+    <definedName name="Качество_товара">Contract!$B$21</definedName>
+    <definedName name="Нарушение_договор">Contract!$B$58</definedName>
+    <definedName name="Поставщик_обязуется">Contract!$B$22</definedName>
+    <definedName name="Транспортная_тара">Contract!$B$23</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -95,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="110">
   <si>
     <t>ДОГОВОР ПОСТАВКИ № 551</t>
   </si>
@@ -1204,6 +1214,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
@@ -1242,9 +1255,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1584,10 +1594,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I99"/>
+  <dimension ref="B1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A62" zoomScale="96" zoomScaleNormal="100" zoomScaleSheetLayoutView="96" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A43" zoomScale="96" zoomScaleNormal="100" zoomScaleSheetLayoutView="96" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1611,16 +1621,16 @@
       </c>
     </row>
     <row r="2" spans="2:9" ht="23.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
     </row>
     <row r="3" spans="2:9" s="18" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="17" t="s">
@@ -1630,22 +1640,22 @@
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
-      <c r="H3" s="64" t="s">
+      <c r="H3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="64"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="2:9" ht="71.349999999999994" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
     </row>
     <row r="5" spans="2:9" ht="5.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="19"/>
@@ -1658,31 +1668,31 @@
       <c r="I5" s="19"/>
     </row>
     <row r="6" spans="2:9" s="18" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="66"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
     </row>
     <row r="7" spans="2:9" ht="29.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
     </row>
     <row r="8" spans="2:9" s="23" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="63" t="s">
         <v>76</v>
       </c>
       <c r="C8" s="59"/>
@@ -1779,7 +1789,7 @@
       <c r="F14" s="39"/>
     </row>
     <row r="15" spans="2:9" s="34" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="63" t="s">
         <v>76</v>
       </c>
       <c r="C15" s="59"/>
@@ -1936,7 +1946,7 @@
       <c r="H26" s="47"/>
       <c r="I26" s="16"/>
     </row>
-    <row r="27" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B27" s="48" t="s">
         <v>104</v>
       </c>
@@ -1948,18 +1958,19 @@
       <c r="H27" s="46"/>
       <c r="I27" s="46"/>
     </row>
-    <row r="28" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B28" s="48" t="s">
         <v>104</v>
       </c>
       <c r="C28" s="48"/>
       <c r="D28" s="46"/>
       <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
       <c r="G28" s="46"/>
       <c r="H28" s="46"/>
       <c r="I28" s="46"/>
     </row>
-    <row r="29" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B29" s="48" t="s">
         <v>104</v>
       </c>
@@ -1971,7 +1982,7 @@
       <c r="H29" s="46"/>
       <c r="I29" s="46"/>
     </row>
-    <row r="30" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B30" s="48" t="s">
         <v>104</v>
       </c>
@@ -1983,7 +1994,7 @@
       <c r="H30" s="46"/>
       <c r="I30" s="46"/>
     </row>
-    <row r="31" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B31" s="48" t="s">
         <v>104</v>
       </c>
@@ -1995,7 +2006,7 @@
       <c r="H31" s="46"/>
       <c r="I31" s="46"/>
     </row>
-    <row r="32" spans="2:9" s="34" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B32" s="48" t="s">
         <v>104</v>
       </c>
@@ -2007,19 +2018,18 @@
       <c r="H32" s="46"/>
       <c r="I32" s="46"/>
     </row>
-    <row r="33" spans="2:9" s="34" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B33" s="48" t="s">
         <v>104</v>
       </c>
       <c r="C33" s="48"/>
       <c r="D33" s="46"/>
       <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
       <c r="G33" s="46"/>
       <c r="H33" s="46"/>
       <c r="I33" s="46"/>
     </row>
-    <row r="34" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B34" s="48" t="s">
         <v>104</v>
       </c>
@@ -2031,7 +2041,7 @@
       <c r="H34" s="46"/>
       <c r="I34" s="46"/>
     </row>
-    <row r="35" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B35" s="48" t="s">
         <v>104</v>
       </c>
@@ -2043,7 +2053,7 @@
       <c r="H35" s="46"/>
       <c r="I35" s="46"/>
     </row>
-    <row r="36" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B36" s="48" t="s">
         <v>104</v>
       </c>
@@ -2055,7 +2065,7 @@
       <c r="H36" s="46"/>
       <c r="I36" s="46"/>
     </row>
-    <row r="37" spans="2:9" s="34" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:9" s="34" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B37" s="48" t="s">
         <v>104</v>
       </c>
@@ -2067,7 +2077,7 @@
       <c r="H37" s="46"/>
       <c r="I37" s="46"/>
     </row>
-    <row r="38" spans="2:9" s="34" customFormat="1" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:9" s="34" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B38" s="48" t="s">
         <v>104</v>
       </c>
@@ -2079,7 +2089,7 @@
       <c r="H38" s="46"/>
       <c r="I38" s="46"/>
     </row>
-    <row r="39" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B39" s="48" t="s">
         <v>104</v>
       </c>
@@ -2091,21 +2101,33 @@
       <c r="H39" s="46"/>
       <c r="I39" s="46"/>
     </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B40" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" s="48"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+    </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B41" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="47"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="47"/>
-    </row>
-    <row r="42" spans="2:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" s="48"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="46"/>
+    </row>
+    <row r="42" spans="2:9" s="34" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B42" s="48" t="s">
-        <v>27</v>
+        <v>104</v>
       </c>
       <c r="C42" s="48"/>
       <c r="D42" s="46"/>
@@ -2115,9 +2137,9 @@
       <c r="H42" s="46"/>
       <c r="I42" s="46"/>
     </row>
-    <row r="43" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:9" s="34" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B43" s="48" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="C43" s="48"/>
       <c r="D43" s="46"/>
@@ -2127,9 +2149,9 @@
       <c r="H43" s="46"/>
       <c r="I43" s="46"/>
     </row>
-    <row r="44" spans="2:9" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B44" s="48" t="s">
-        <v>29</v>
+        <v>104</v>
       </c>
       <c r="C44" s="48"/>
       <c r="D44" s="46"/>
@@ -2139,46 +2161,45 @@
       <c r="H44" s="46"/>
       <c r="I44" s="46"/>
     </row>
-    <row r="45" spans="2:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="C45" s="48"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
-    </row>
-    <row r="46" spans="2:9" ht="86.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="C46" s="48"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="46"/>
-      <c r="G46" s="46"/>
-      <c r="H46" s="46"/>
-      <c r="I46" s="46"/>
-    </row>
-    <row r="47" spans="2:9" ht="12.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B48" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" s="16"/>
-      <c r="D48" s="47"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="47"/>
-      <c r="H48" s="47"/>
-      <c r="I48" s="47"/>
-    </row>
-    <row r="49" spans="2:9" s="49" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B46" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="16"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="47"/>
+      <c r="G46" s="47"/>
+      <c r="H46" s="47"/>
+      <c r="I46" s="47"/>
+    </row>
+    <row r="47" spans="2:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B47" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" s="48"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
+    </row>
+    <row r="48" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B48" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="48"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="46"/>
+    </row>
+    <row r="49" spans="2:9" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B49" s="48" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C49" s="48"/>
       <c r="D49" s="46"/>
@@ -2188,21 +2209,21 @@
       <c r="H49" s="46"/>
       <c r="I49" s="46"/>
     </row>
-    <row r="50" spans="2:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B50" s="48" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C50" s="48"/>
-      <c r="D50" s="44"/>
-      <c r="E50" s="44"/>
-      <c r="F50" s="44"/>
-      <c r="G50" s="44"/>
-      <c r="H50" s="44"/>
-      <c r="I50" s="44"/>
-    </row>
-    <row r="51" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
+    </row>
+    <row r="51" spans="2:9" ht="86.35" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B51" s="48" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C51" s="48"/>
       <c r="D51" s="46"/>
@@ -2212,33 +2233,22 @@
       <c r="H51" s="46"/>
       <c r="I51" s="46"/>
     </row>
-    <row r="52" spans="2:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="C52" s="48"/>
-      <c r="D52" s="46"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="46"/>
-      <c r="G52" s="46"/>
-      <c r="H52" s="46"/>
-      <c r="I52" s="46"/>
-    </row>
-    <row r="53" spans="2:9" ht="41.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="C53" s="48"/>
-      <c r="D53" s="46"/>
-      <c r="E53" s="46"/>
-      <c r="F53" s="46"/>
-      <c r="G53" s="46"/>
-      <c r="H53" s="46"/>
-      <c r="I53" s="46"/>
-    </row>
-    <row r="54" spans="2:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:9" ht="12.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B53" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C53" s="16"/>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="47"/>
+      <c r="H53" s="47"/>
+      <c r="I53" s="47"/>
+    </row>
+    <row r="54" spans="2:9" s="49" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B54" s="48" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C54" s="48"/>
       <c r="D54" s="46"/>
@@ -2248,22 +2258,33 @@
       <c r="H54" s="46"/>
       <c r="I54" s="46"/>
     </row>
-    <row r="55" spans="2:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B56" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C56" s="16"/>
-      <c r="D56" s="47"/>
-      <c r="E56" s="47"/>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="47"/>
-      <c r="I56" s="47"/>
-    </row>
-    <row r="57" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B55" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C55" s="48"/>
+      <c r="D55" s="44"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="44"/>
+      <c r="H55" s="44"/>
+      <c r="I55" s="44"/>
+    </row>
+    <row r="56" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B56" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C56" s="48"/>
+      <c r="D56" s="46"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="46"/>
+      <c r="H56" s="46"/>
+      <c r="I56" s="46"/>
+    </row>
+    <row r="57" spans="2:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B57" s="48" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C57" s="48"/>
       <c r="D57" s="46"/>
@@ -2273,51 +2294,46 @@
       <c r="H57" s="46"/>
       <c r="I57" s="46"/>
     </row>
-    <row r="58" spans="2:9" s="44" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:9" ht="41.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B58" s="48" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C58" s="48"/>
-    </row>
-    <row r="59" spans="2:9" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D58" s="46"/>
+      <c r="E58" s="46"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="46"/>
+      <c r="I58" s="46"/>
+    </row>
+    <row r="59" spans="2:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B59" s="48" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C59" s="48"/>
-      <c r="D59" s="44"/>
-      <c r="E59" s="44"/>
-      <c r="F59" s="44"/>
-      <c r="G59" s="44"/>
-      <c r="H59" s="44"/>
-      <c r="I59" s="44"/>
-    </row>
-    <row r="60" spans="2:9" s="34" customFormat="1" ht="42.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B60" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="C60" s="48"/>
-      <c r="D60" s="46"/>
-      <c r="E60" s="46"/>
-      <c r="F60" s="46"/>
-      <c r="G60" s="46"/>
-      <c r="H60" s="46"/>
-      <c r="I60" s="46"/>
-    </row>
-    <row r="61" spans="2:9" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B61" s="48" t="s">
-        <v>48</v>
-      </c>
-      <c r="C61" s="48"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="44"/>
-      <c r="F61" s="44"/>
-      <c r="G61" s="44"/>
-      <c r="H61" s="44"/>
-      <c r="I61" s="44"/>
-    </row>
-    <row r="62" spans="2:9" s="49" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="D59" s="46"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="46"/>
+      <c r="H59" s="46"/>
+      <c r="I59" s="46"/>
+    </row>
+    <row r="60" spans="2:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B61" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" s="16"/>
+      <c r="D61" s="47"/>
+      <c r="E61" s="47"/>
+      <c r="F61" s="47"/>
+      <c r="G61" s="47"/>
+      <c r="H61" s="47"/>
+      <c r="I61" s="47"/>
+    </row>
+    <row r="62" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B62" s="48" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C62" s="48"/>
       <c r="D62" s="46"/>
@@ -2327,225 +2343,279 @@
       <c r="H62" s="46"/>
       <c r="I62" s="46"/>
     </row>
-    <row r="63" spans="2:9" s="34" customFormat="1" ht="44.35" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="2:9" s="44" customFormat="1" ht="16.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B63" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="C63" s="48"/>
+    </row>
+    <row r="64" spans="2:9" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B64" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C64" s="48"/>
+      <c r="D64" s="44"/>
+      <c r="E64" s="44"/>
+      <c r="F64" s="44"/>
+      <c r="G64" s="44"/>
+      <c r="H64" s="44"/>
+      <c r="I64" s="44"/>
+    </row>
+    <row r="65" spans="2:9" s="34" customFormat="1" ht="42.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B65" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="C65" s="48"/>
+      <c r="D65" s="46"/>
+      <c r="E65" s="46"/>
+      <c r="F65" s="46"/>
+      <c r="G65" s="46"/>
+      <c r="H65" s="46"/>
+      <c r="I65" s="46"/>
+    </row>
+    <row r="66" spans="2:9" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B66" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="C66" s="48"/>
+      <c r="D66" s="44"/>
+      <c r="E66" s="44"/>
+      <c r="F66" s="44"/>
+      <c r="G66" s="44"/>
+      <c r="H66" s="44"/>
+      <c r="I66" s="44"/>
+    </row>
+    <row r="67" spans="2:9" s="49" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B67" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C67" s="48"/>
+      <c r="D67" s="46"/>
+      <c r="E67" s="46"/>
+      <c r="F67" s="46"/>
+      <c r="G67" s="46"/>
+      <c r="H67" s="46"/>
+      <c r="I67" s="46"/>
+    </row>
+    <row r="68" spans="2:9" s="34" customFormat="1" ht="44.35" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B68" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="C63" s="48"/>
-      <c r="D63" s="46"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="46"/>
-      <c r="G63" s="46"/>
-      <c r="H63" s="46"/>
-      <c r="I63" s="46"/>
-    </row>
-    <row r="64" spans="2:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="65" spans="2:9" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B65" s="20" t="s">
+      <c r="C68" s="48"/>
+      <c r="D68" s="46"/>
+      <c r="E68" s="46"/>
+      <c r="F68" s="46"/>
+      <c r="G68" s="46"/>
+      <c r="H68" s="46"/>
+      <c r="I68" s="46"/>
+    </row>
+    <row r="69" spans="2:9" ht="14.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="70" spans="2:9" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B70" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C65" s="20"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
-      <c r="I65" s="17"/>
-    </row>
-    <row r="66" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B66" s="51" t="s">
+      <c r="C70" s="20"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="17"/>
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="17"/>
+    </row>
+    <row r="71" spans="2:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B71" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="C66" s="51"/>
-      <c r="D66" s="47" t="s">
+      <c r="C71" s="51"/>
+      <c r="D71" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="E66" s="52"/>
-      <c r="G66" s="51" t="s">
+      <c r="E71" s="52"/>
+      <c r="G71" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="H66" s="47"/>
-      <c r="I66" s="47" t="s">
+      <c r="H71" s="47"/>
+      <c r="I71" s="47" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="67" spans="2:9" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B67" s="56" t="s">
+    <row r="72" spans="2:9" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B72" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="C67" s="56"/>
-      <c r="D67" s="45"/>
-      <c r="E67" s="45"/>
-      <c r="G67" s="56" t="s">
+      <c r="C72" s="56"/>
+      <c r="D72" s="45"/>
+      <c r="E72" s="45"/>
+      <c r="G72" s="56" t="s">
         <v>100</v>
-      </c>
-      <c r="H67" s="34"/>
-      <c r="I67" s="34"/>
-    </row>
-    <row r="68" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B68" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="C68" s="56"/>
-      <c r="D68" s="45"/>
-      <c r="E68" s="45"/>
-      <c r="G68" s="56" t="s">
-        <v>103</v>
-      </c>
-      <c r="H68" s="45"/>
-      <c r="I68" s="45"/>
-    </row>
-    <row r="69" spans="2:9" ht="12.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B69" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="C69" s="56"/>
-      <c r="D69" s="57"/>
-      <c r="E69" s="45"/>
-      <c r="G69" s="56" t="s">
-        <v>94</v>
-      </c>
-      <c r="H69" s="45"/>
-      <c r="I69" s="45"/>
-    </row>
-    <row r="70" spans="2:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B70" s="56" t="s">
-        <v>95</v>
-      </c>
-      <c r="C70" s="56"/>
-      <c r="D70" s="45"/>
-      <c r="E70" s="45"/>
-      <c r="G70" s="56" t="s">
-        <v>102</v>
-      </c>
-      <c r="H70" s="45"/>
-      <c r="I70" s="45"/>
-    </row>
-    <row r="71" spans="2:9" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="B71" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="C71" s="56"/>
-      <c r="D71" s="45"/>
-      <c r="E71" s="53"/>
-      <c r="G71" s="56" t="s">
-        <v>101</v>
-      </c>
-      <c r="H71" s="45"/>
-      <c r="I71" s="45"/>
-    </row>
-    <row r="72" spans="2:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B72" s="56" t="s">
-        <v>99</v>
-      </c>
-      <c r="C72" s="56"/>
-      <c r="D72" s="34"/>
-      <c r="G72" s="56" t="s">
-        <v>92</v>
       </c>
       <c r="H72" s="34"/>
       <c r="I72" s="34"/>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="73" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B73" s="56" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C73" s="56"/>
       <c r="D73" s="45"/>
       <c r="E73" s="45"/>
       <c r="G73" s="56" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="H73" s="45"/>
       <c r="I73" s="45"/>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="74" spans="2:9" ht="12.85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B74" s="56" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="C74" s="56"/>
-      <c r="D74" s="45"/>
+      <c r="D74" s="57"/>
       <c r="E74" s="45"/>
       <c r="G74" s="56" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H74" s="45"/>
       <c r="I74" s="45"/>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.4">
+    <row r="75" spans="2:9" ht="13.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B75" s="56" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="C75" s="56"/>
       <c r="D75" s="45"/>
       <c r="E75" s="45"/>
       <c r="G75" s="56" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="H75" s="45"/>
       <c r="I75" s="45"/>
     </row>
-    <row r="77" spans="2:9" ht="30.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="78" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B78" s="61" t="s">
+    <row r="76" spans="2:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B76" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="C76" s="56"/>
+      <c r="D76" s="45"/>
+      <c r="E76" s="53"/>
+      <c r="G76" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="H76" s="45"/>
+      <c r="I76" s="45"/>
+    </row>
+    <row r="77" spans="2:9" ht="31.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B77" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="C77" s="56"/>
+      <c r="D77" s="34"/>
+      <c r="G77" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="H77" s="34"/>
+      <c r="I77" s="34"/>
+    </row>
+    <row r="78" spans="2:9" ht="15.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B78" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="C78" s="56"/>
+      <c r="D78" s="45"/>
+      <c r="E78" s="45"/>
+      <c r="G78" s="56" t="s">
+        <v>71</v>
+      </c>
+      <c r="H78" s="45"/>
+      <c r="I78" s="45"/>
+    </row>
+    <row r="79" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B79" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="C79" s="56"/>
+      <c r="D79" s="45"/>
+      <c r="E79" s="45"/>
+      <c r="G79" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="H79" s="45"/>
+      <c r="I79" s="45"/>
+    </row>
+    <row r="80" spans="2:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B80" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="C80" s="56"/>
+      <c r="D80" s="45"/>
+      <c r="E80" s="45"/>
+      <c r="G80" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="H80" s="45"/>
+      <c r="I80" s="45"/>
+    </row>
+    <row r="82" spans="2:9" ht="30.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="83" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B83" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="C78" s="18" t="s">
+      <c r="C83" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D78" s="61"/>
-      <c r="E78" s="37"/>
-      <c r="G78" s="61" t="s">
+      <c r="D83" s="61"/>
+      <c r="E83" s="37"/>
+      <c r="G83" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="H78" s="61"/>
-      <c r="I78" s="61"/>
-    </row>
-    <row r="79" spans="2:9" ht="20.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C79" s="18" t="s">
+      <c r="H83" s="61"/>
+      <c r="I83" s="61"/>
+    </row>
+    <row r="84" spans="2:9" ht="20.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C84" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D79" s="54"/>
-      <c r="G79" s="55"/>
-      <c r="H79" s="55"/>
-      <c r="I79" s="55"/>
-    </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B80" s="60" t="s">
+      <c r="D84" s="54"/>
+      <c r="G84" s="55"/>
+      <c r="H84" s="55"/>
+      <c r="I84" s="55"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B85" s="60" t="s">
         <v>74</v>
       </c>
-      <c r="C80" s="60"/>
-      <c r="D80" s="60"/>
-      <c r="E80" s="37"/>
-      <c r="G80" s="60" t="s">
+      <c r="C85" s="60"/>
+      <c r="D85" s="60"/>
+      <c r="E85" s="37"/>
+      <c r="G85" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="H80" s="60"/>
-      <c r="I80" s="60"/>
-    </row>
-    <row r="81" spans="9:9" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="I81" s="15" t="s">
+      <c r="H85" s="60"/>
+      <c r="I85" s="60"/>
+    </row>
+    <row r="86" spans="2:9" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="I86" s="15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="82" spans="9:9" ht="35.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="83" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="84" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="85" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="86" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="87" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="88" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="89" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="90" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="91" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="92" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="93" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="94" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="95" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="96" spans="9:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="87" spans="2:9" ht="35.75" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="88" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="89" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="90" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="91" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="92" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="93" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="94" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="95" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="96" spans="2:9" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="97" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="98" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="99" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="100" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="101" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="102" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="103" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="104" ht="0.85" customHeight="1" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B4:I4"/>
@@ -2558,7 +2628,7 @@
   <pageMargins left="7.874015748031496E-2" right="7.874015748031496E-2" top="0.19685039370078741" bottom="0.19685039370078741" header="0.11811023622047245" footer="0"/>
   <pageSetup paperSize="9" scale="77" fitToHeight="2" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="44" max="8" man="1"/>
+    <brk id="49" max="8" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -2582,11 +2652,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="23.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
     </row>
     <row r="2" spans="2:4" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
@@ -2597,54 +2667,54 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="99.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
     </row>
     <row r="5" spans="2:4" ht="26.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
     </row>
     <row r="6" spans="2:4" s="7" customFormat="1" ht="35.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
     </row>
     <row r="7" spans="2:4" s="8" customFormat="1" ht="35.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
     </row>
     <row r="9" spans="2:4" ht="12" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="2:4" ht="14.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B11" s="3" t="s">
@@ -2652,291 +2722,291 @@
       </c>
     </row>
     <row r="12" spans="2:4" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
     </row>
     <row r="13" spans="2:4" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
     </row>
     <row r="14" spans="2:4" s="7" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
     </row>
     <row r="16" spans="2:4" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="71" t="s">
+      <c r="B16" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
     </row>
     <row r="17" spans="2:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="70" t="s">
+      <c r="B17" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
     </row>
     <row r="18" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="68"/>
-      <c r="D18" s="68"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B19" s="68" t="s">
+      <c r="B19" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="73"/>
-      <c r="D20" s="73"/>
+      <c r="C20" s="74"/>
+      <c r="D20" s="74"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B21" s="73" t="s">
+      <c r="B21" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
+      <c r="C21" s="74"/>
+      <c r="D21" s="74"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B23" s="71" t="s">
+      <c r="B23" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
     </row>
     <row r="24" spans="2:4" ht="39.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="68" t="s">
+      <c r="B24" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
     </row>
     <row r="25" spans="2:4" s="8" customFormat="1" ht="27.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="68" t="s">
+      <c r="B25" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="68"/>
-      <c r="D25" s="68"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
     </row>
     <row r="26" spans="2:4" s="8" customFormat="1" ht="28.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="68" t="s">
+      <c r="B26" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="68"/>
-      <c r="D26" s="68"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
     </row>
     <row r="27" spans="2:4" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="69"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B28" s="73" t="s">
+      <c r="B28" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="73"/>
-      <c r="D28" s="73"/>
+      <c r="C28" s="74"/>
+      <c r="D28" s="74"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B29" s="73" t="s">
+      <c r="B29" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="73"/>
-      <c r="D29" s="73"/>
+      <c r="C29" s="74"/>
+      <c r="D29" s="74"/>
     </row>
     <row r="30" spans="2:4" s="8" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="68" t="s">
+      <c r="B30" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="68"/>
-      <c r="D30" s="68"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
     </row>
     <row r="31" spans="2:4" s="8" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="68" t="s">
+      <c r="B31" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="68"/>
-      <c r="D31" s="68"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B32" s="73" t="s">
+      <c r="B32" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="73"/>
-      <c r="D32" s="73"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="74"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B34" s="71" t="s">
+      <c r="B34" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="72"/>
     </row>
     <row r="35" spans="2:4" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="68" t="s">
+      <c r="B35" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="68"/>
-      <c r="D35" s="68"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
     </row>
     <row r="36" spans="2:4" ht="27.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="68" t="s">
+      <c r="B36" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="68"/>
-      <c r="D36" s="68"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="69"/>
     </row>
     <row r="37" spans="2:4" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="68" t="s">
+      <c r="B37" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
     </row>
     <row r="38" spans="2:4" ht="66" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="72" t="s">
+      <c r="B38" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="72"/>
-      <c r="D38" s="72"/>
+      <c r="C38" s="73"/>
+      <c r="D38" s="73"/>
     </row>
     <row r="39" spans="2:4" ht="113.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="70" t="s">
+      <c r="B39" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="70"/>
-      <c r="D39" s="70"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="71"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B41" s="71" t="s">
+      <c r="B41" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
+      <c r="C41" s="72"/>
+      <c r="D41" s="72"/>
     </row>
     <row r="42" spans="2:4" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="68" t="s">
+      <c r="B42" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="68"/>
-      <c r="D42" s="68"/>
+      <c r="C42" s="69"/>
+      <c r="D42" s="69"/>
     </row>
     <row r="43" spans="2:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="68" t="s">
+      <c r="B43" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="68"/>
-      <c r="D43" s="68"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="69"/>
     </row>
     <row r="44" spans="2:4" ht="30.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="70" t="s">
+      <c r="B44" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="70"/>
-      <c r="D44" s="70"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="71"/>
     </row>
     <row r="45" spans="2:4" ht="42.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="70" t="s">
+      <c r="B45" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="70"/>
-      <c r="D45" s="70"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="71"/>
     </row>
     <row r="46" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="70" t="s">
+      <c r="B46" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="70"/>
-      <c r="D46" s="70"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="71"/>
     </row>
     <row r="47" spans="2:4" ht="39" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="70" t="s">
+      <c r="B47" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="70"/>
-      <c r="D47" s="70"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="71"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B49" s="71" t="s">
+      <c r="B49" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="71"/>
-      <c r="D49" s="71"/>
+      <c r="C49" s="72"/>
+      <c r="D49" s="72"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B50" s="70" t="s">
+      <c r="B50" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="70"/>
-      <c r="D50" s="70"/>
+      <c r="C50" s="71"/>
+      <c r="D50" s="71"/>
     </row>
     <row r="51" spans="2:4" s="9" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="70" t="s">
+      <c r="B51" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="70"/>
-      <c r="D51" s="70"/>
+      <c r="C51" s="71"/>
+      <c r="D51" s="71"/>
     </row>
     <row r="52" spans="2:4" ht="26.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="68" t="s">
+      <c r="B52" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="68"/>
-      <c r="D52" s="68"/>
+      <c r="C52" s="69"/>
+      <c r="D52" s="69"/>
     </row>
     <row r="53" spans="2:4" s="8" customFormat="1" ht="36.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="68" t="s">
+      <c r="B53" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="68"/>
-      <c r="D53" s="68"/>
+      <c r="C53" s="69"/>
+      <c r="D53" s="69"/>
     </row>
     <row r="54" spans="2:4" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B54" s="70" t="s">
+      <c r="B54" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="70"/>
-      <c r="D54" s="70"/>
+      <c r="C54" s="71"/>
+      <c r="D54" s="71"/>
     </row>
     <row r="55" spans="2:4" s="5" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="68" t="s">
+      <c r="B55" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="68"/>
-      <c r="D55" s="68"/>
+      <c r="C55" s="69"/>
+      <c r="D55" s="69"/>
     </row>
     <row r="56" spans="2:4" s="8" customFormat="1" ht="51.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="68" t="s">
+      <c r="B56" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="68"/>
-      <c r="D56" s="68"/>
+      <c r="C56" s="69"/>
+      <c r="D56" s="69"/>
     </row>
     <row r="58" spans="2:4" s="6" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="69" t="s">
+      <c r="B58" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="69"/>
-      <c r="D58" s="69"/>
+      <c r="C58" s="70"/>
+      <c r="D58" s="70"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B59" s="10" t="s">

</xml_diff>